<commit_message>
rename first page of excel book
</commit_message>
<xml_diff>
--- a/CHC-indentification.xlsx
+++ b/CHC-indentification.xlsx
@@ -6,16 +6,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\Documentos\PhD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CHC-identification_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D624ED-1051-4FFF-B4CF-07C8EFFAA647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="097FGWlWYFTK/0FG2lB+72shyRPGqCqZjG+vN/O7jEZcbY1z+zoGRSy1D8+Ave/ZEAB2ubKfltV0f1awL1hlGA==" workbookSaltValue="wlTpuOApVMHVSYv8mkR95A==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED966C7-54E3-42A4-8D41-3FFAC1F64F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Identification" sheetId="1" r:id="rId1"/>
+    <sheet name="CHC-Identification" sheetId="1" r:id="rId1"/>
     <sheet name="Carlson(1998)-methyl alkanes" sheetId="3" r:id="rId2"/>
     <sheet name="post-DMDS" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -1680,875 +1679,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="176">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="52">
     <dxf>
       <fill>
         <patternFill>
@@ -3344,7 +2475,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4643,262 +3774,262 @@
     <mergeCell ref="F13:Q13"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C31">
-    <cfRule type="cellIs" dxfId="111" priority="201" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="201" operator="greaterThanOrEqual">
       <formula>$B$3-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D31">
-    <cfRule type="cellIs" dxfId="110" priority="200" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="200" operator="greaterThanOrEqual">
       <formula>$B$4-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E31">
-    <cfRule type="cellIs" dxfId="109" priority="198" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="198" operator="greaterThanOrEqual">
       <formula>$B$5-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="expression" dxfId="108" priority="108">
+    <cfRule type="expression" dxfId="48" priority="108">
       <formula>COUNTIF($B$1,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="107" priority="97">
+    <cfRule type="expression" dxfId="47" priority="97">
       <formula>COUNTIF(F$6:G$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="106" priority="90">
+    <cfRule type="expression" dxfId="46" priority="90">
       <formula>COUNTIF(J6:K6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="105" priority="89">
+    <cfRule type="expression" dxfId="45" priority="89">
       <formula>COUNTIF(L6:M6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="104" priority="88">
+    <cfRule type="expression" dxfId="44" priority="88">
       <formula>COUNTIF(N6:O6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="103" priority="87">
+    <cfRule type="expression" dxfId="43" priority="87">
       <formula>COUNTIF(P6:Q6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="102" priority="86">
+    <cfRule type="expression" dxfId="42" priority="86">
       <formula>COUNTIF(F8:G8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="101" priority="68">
+    <cfRule type="expression" dxfId="41" priority="68">
       <formula>COUNTIF(F10:G10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="100" priority="67">
+    <cfRule type="expression" dxfId="40" priority="67">
       <formula>COUNTIF(F12:G12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="99" priority="65">
+    <cfRule type="expression" dxfId="39" priority="65">
       <formula>COUNTIF(H$6:I$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="98" priority="60">
+    <cfRule type="expression" dxfId="38" priority="60">
       <formula>COUNTIF(H8:I8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="97" priority="57">
+    <cfRule type="expression" dxfId="37" priority="57">
       <formula>COUNTIF(H10:I10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="96" priority="56">
+    <cfRule type="expression" dxfId="36" priority="56">
       <formula>COUNTIF(H12:I12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="95" priority="54">
+    <cfRule type="expression" dxfId="35" priority="54">
       <formula>COUNTIF(J10:K10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="94" priority="53">
+    <cfRule type="expression" dxfId="34" priority="53">
       <formula>COUNTIF(J12:K12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="93" priority="52">
+    <cfRule type="expression" dxfId="33" priority="52">
       <formula>COUNTIF(J8:K8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="92" priority="50">
+    <cfRule type="expression" dxfId="32" priority="50">
       <formula>COUNTIF(L8:M8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="expression" dxfId="91" priority="49">
+    <cfRule type="expression" dxfId="31" priority="49">
       <formula>COUNTIF(L10:M10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="90" priority="48">
+    <cfRule type="expression" dxfId="30" priority="48">
       <formula>COUNTIF(L12:M12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="89" priority="47">
+    <cfRule type="expression" dxfId="29" priority="47">
       <formula>COUNTIF(N8:O8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="88" priority="46">
+    <cfRule type="expression" dxfId="28" priority="46">
       <formula>COUNTIF(N10:O10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="expression" dxfId="87" priority="45">
+    <cfRule type="expression" dxfId="27" priority="45">
       <formula>COUNTIF(N12:O12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="expression" dxfId="86" priority="44">
+    <cfRule type="expression" dxfId="26" priority="44">
       <formula>COUNTIF(P8:Q8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9">
-    <cfRule type="expression" dxfId="85" priority="43">
+    <cfRule type="expression" dxfId="25" priority="43">
       <formula>COUNTIF(P10:Q10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="expression" dxfId="84" priority="42">
+    <cfRule type="expression" dxfId="24" priority="42">
       <formula>COUNTIF(P12:Q12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16">
-    <cfRule type="expression" dxfId="83" priority="41">
+    <cfRule type="expression" dxfId="23" priority="41">
       <formula>COUNTIF($G$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:I18">
-    <cfRule type="expression" dxfId="82" priority="36">
+    <cfRule type="expression" dxfId="22" priority="36">
       <formula>COUNTIF($I$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:I20">
-    <cfRule type="expression" dxfId="81" priority="35">
+    <cfRule type="expression" dxfId="21" priority="35">
       <formula>COUNTIF($I$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="expression" dxfId="80" priority="34">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>COUNTIF($I$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18">
-    <cfRule type="expression" dxfId="79" priority="32">
+    <cfRule type="expression" dxfId="19" priority="32">
       <formula>COUNTIF($K$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="expression" dxfId="78" priority="31">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>COUNTIF($K$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="expression" dxfId="77" priority="30">
+    <cfRule type="expression" dxfId="17" priority="30">
       <formula>COUNTIF($K$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:M16">
-    <cfRule type="expression" dxfId="76" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>COUNTIF($M$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:O16">
-    <cfRule type="expression" dxfId="75" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>COUNTIF($O$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:Q16">
-    <cfRule type="expression" dxfId="74" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>COUNTIF($Q$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:M18">
-    <cfRule type="expression" dxfId="73" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>COUNTIF($M$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:O18">
-    <cfRule type="expression" dxfId="72" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>COUNTIF($O$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="71" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>COUNTIF($Q$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:M20">
-    <cfRule type="expression" dxfId="70" priority="13">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>COUNTIF($M$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:O20">
-    <cfRule type="expression" dxfId="69" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>COUNTIF($O$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:Q20">
-    <cfRule type="expression" dxfId="68" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>COUNTIF($Q$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:M22">
-    <cfRule type="expression" dxfId="67" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>COUNTIF($M$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:O22">
-    <cfRule type="expression" dxfId="66" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>COUNTIF($O$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:Q22">
-    <cfRule type="expression" dxfId="65" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>COUNTIF($Q$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:G18">
-    <cfRule type="expression" dxfId="64" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>COUNTIF($G$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:G20">
-    <cfRule type="expression" dxfId="63" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>COUNTIF($G$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:G22">
-    <cfRule type="expression" dxfId="62" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>COUNTIF($G$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:I16">
-    <cfRule type="expression" dxfId="61" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>COUNTIF($I$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16">
-    <cfRule type="expression" dxfId="60" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF($K$15,"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correct the conditional formating of one of the dimethyl cells
</commit_message>
<xml_diff>
--- a/CHC-indentification.xlsx
+++ b/CHC-indentification.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CHC-identification_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED966C7-54E3-42A4-8D41-3FFAC1F64F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB991A02-D806-4AFD-BB70-4291026E5FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
   </bookViews>
@@ -2475,7 +2475,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3925,111 +3925,111 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:I20">
     <cfRule type="expression" dxfId="21" priority="35">
+      <formula>COUNTIF($I$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:I22">
+    <cfRule type="expression" dxfId="0" priority="34">
       <formula>COUNTIF($I$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:I22">
-    <cfRule type="expression" dxfId="20" priority="34">
-      <formula>COUNTIF($I$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18">
-    <cfRule type="expression" dxfId="19" priority="32">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>COUNTIF($K$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="expression" dxfId="18" priority="31">
+    <cfRule type="expression" dxfId="19" priority="31">
       <formula>COUNTIF($K$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="expression" dxfId="17" priority="30">
+    <cfRule type="expression" dxfId="18" priority="30">
       <formula>COUNTIF($K$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:M16">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="17" priority="17">
       <formula>COUNTIF($M$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:O16">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="16" priority="16">
       <formula>COUNTIF($O$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:Q16">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>COUNTIF($Q$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:M18">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>COUNTIF($M$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:O18">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>COUNTIF($O$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>COUNTIF($Q$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:M20">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>COUNTIF($M$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:O20">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>COUNTIF($O$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:Q20">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>COUNTIF($Q$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:M22">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>COUNTIF($M$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:O22">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>COUNTIF($O$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:Q22">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>COUNTIF($Q$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:G18">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>COUNTIF($G$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:G20">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>COUNTIF($G$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:G22">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>COUNTIF($G$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:I16">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>COUNTIF($I$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>COUNTIF($K$15,"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correct calculation of second methylation position of dimethyl-branched alkanes
</commit_message>
<xml_diff>
--- a/CHC-indentification.xlsx
+++ b/CHC-indentification.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CHC-identification_tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Trabajo\Proyectos\Chemical Ecology\CHC-identification_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB991A02-D806-4AFD-BB70-4291026E5FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80038E6-A19A-4942-93F3-1AFAC2A6CC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
   </bookViews>
   <sheets>
     <sheet name="CHC-Identification" sheetId="1" r:id="rId1"/>
@@ -1485,7 +1485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1496,10 +1496,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1514,31 +1514,31 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1547,13 +1547,13 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1597,15 +1597,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2464,7 +2455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2474,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FD13C8-9C57-4E7C-B7EE-A41A7F7BBBB9}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2491,47 +2482,47 @@
         <v>3</v>
       </c>
       <c r="B1" s="24"/>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="50" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="51"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="47" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="49"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2550,20 +2541,20 @@
       <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="55"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="52"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2584,24 +2575,24 @@
         <f>D4-2</f>
         <v>39</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57" t="s">
+      <c r="G4" s="54"/>
+      <c r="H4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="59" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="61"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="58"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2640,7 +2631,7 @@
         <v>6</v>
       </c>
       <c r="K5" s="18" t="e">
-        <f>MIN(J36:K36)</f>
+        <f>MAX(J36:K36)</f>
         <v>#N/A</v>
       </c>
       <c r="L5" s="30" t="s">
@@ -2734,7 +2725,7 @@
         <v>6</v>
       </c>
       <c r="K7" s="18" t="e">
-        <f>MIN(J37:K37)</f>
+        <f>MAX(J37:K37)</f>
         <v>#N/A</v>
       </c>
       <c r="L7" s="30" t="s">
@@ -2821,7 +2812,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="18" t="e">
-        <f>MIN(J38:K38)</f>
+        <f>MAX(J38:K38)</f>
         <v>#N/A</v>
       </c>
       <c r="L9" s="30" t="s">
@@ -2901,7 +2892,7 @@
         <v>6</v>
       </c>
       <c r="K11" s="18" t="e">
-        <f>MIN(J39:K39)</f>
+        <f>MAX(J39:K39)</f>
         <v>#N/A</v>
       </c>
       <c r="L11" s="30" t="s">
@@ -2963,20 +2954,20 @@
         <f t="shared" si="8"/>
         <v>165</v>
       </c>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="55"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="52"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="11">
@@ -2990,24 +2981,24 @@
         <f t="shared" si="9"/>
         <v>179</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57" t="s">
+      <c r="G14" s="54"/>
+      <c r="H14" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="59" t="s">
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="61"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="C15" s="11">
@@ -3062,7 +3053,7 @@
         <f>_xlfn.CONCAT((G15*14+14+1),"|",(G15*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="G16" s="39" t="str">
+      <c r="G16" s="18" t="str">
         <f>_xlfn.CONCAT(($B$6-(G15*14+14+1)+28), "|", ($B$6-(G15*14+14+1)+28)-1)</f>
         <v>29|28</v>
       </c>
@@ -3070,7 +3061,7 @@
         <f>_xlfn.CONCAT((I15*14+14+1),"|",(I15*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="I16" s="39" t="str">
+      <c r="I16" s="18" t="str">
         <f>_xlfn.CONCAT(($B$7-(I15*14+14+1)+28), "|", ($B$7-(I15*14+14+1)+28)-1)</f>
         <v>43|42</v>
       </c>
@@ -3078,7 +3069,7 @@
         <f>_xlfn.CONCAT((K15*14+(14*2)+1),"|",(K15*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="K16" s="39" t="str">
+      <c r="K16" s="18" t="str">
         <f>_xlfn.CONCAT(($B$7-(K15*14+1)),"|",($B$7-(K15*14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3086,7 +3077,7 @@
         <f>_xlfn.CONCAT((M15*14+14+1),"|",(M15*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="M16" s="39" t="str">
+      <c r="M16" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(M15*14+14+1)+28), "|", ($B$8-(M15*14+14+1)+28)-1)</f>
         <v>57|56</v>
       </c>
@@ -3094,7 +3085,7 @@
         <f>_xlfn.CONCAT((O15*14+(14*2)+1),"|",(O15*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="O16" s="39" t="str">
+      <c r="O16" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(O15*14+1)),"|",($B$8-(O15*14+1)-1))</f>
         <v>43|42</v>
       </c>
@@ -3102,7 +3093,7 @@
         <f>_xlfn.CONCAT((Q15*14+(14*3)+1),"|",(Q15*14+(14*3)))</f>
         <v>43|42</v>
       </c>
-      <c r="Q16" s="41" t="str">
+      <c r="Q16" s="21" t="str">
         <f>_xlfn.CONCAT(($B$8-(Q15*14+14+1)),"|",($B$8-(Q15*14+14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3160,7 +3151,7 @@
         <f>_xlfn.CONCAT((G17*14+14+1),"|",(G17*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="G18" s="39" t="str">
+      <c r="G18" s="18" t="str">
         <f>_xlfn.CONCAT(($B$6-(G17*14+14+1)+28), "|", ($B$6-(G17*14+14+1)+28)-1)</f>
         <v>29|28</v>
       </c>
@@ -3168,7 +3159,7 @@
         <f>_xlfn.CONCAT((I17*14+14+1),"|",(I17*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="I18" s="39" t="str">
+      <c r="I18" s="18" t="str">
         <f>_xlfn.CONCAT(($B$7-(I17*14+14+1)+28), "|", ($B$7-(I17*14+14+1)+28)-1)</f>
         <v>43|42</v>
       </c>
@@ -3176,7 +3167,7 @@
         <f>_xlfn.CONCAT((K17*14+(14*2)+1),"|",(K17*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="K18" s="40" t="str">
+      <c r="K18" s="10" t="str">
         <f>_xlfn.CONCAT(($B$7-(K17*14+1)),"|",($B$7-(K17*14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3184,7 +3175,7 @@
         <f>_xlfn.CONCAT((M17*14+14+1),"|",(M17*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="M18" s="39" t="str">
+      <c r="M18" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(M17*14+14+1)+28), "|", ($B$8-(M17*14+14+1)+28)-1)</f>
         <v>57|56</v>
       </c>
@@ -3192,7 +3183,7 @@
         <f>_xlfn.CONCAT((O17*14+(14*2)+1),"|",(O17*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="O18" s="39" t="str">
+      <c r="O18" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(O17*14+1)),"|",($B$8-(O17*14+1)-1))</f>
         <v>43|42</v>
       </c>
@@ -3200,7 +3191,7 @@
         <f>_xlfn.CONCAT((Q17*14+(14*3)+1),"|",(Q17*14+(14*3)))</f>
         <v>43|42</v>
       </c>
-      <c r="Q18" s="41" t="str">
+      <c r="Q18" s="21" t="str">
         <f>_xlfn.CONCAT(($B$8-(Q17*14+14+1)),"|",($B$8-(Q17*14+14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3258,7 +3249,7 @@
         <f>_xlfn.CONCAT((G19*14+14+1),"|",(G19*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="G20" s="39" t="str">
+      <c r="G20" s="18" t="str">
         <f>_xlfn.CONCAT(($B$6-(G19*14+14+1)+28), "|", ($B$6-(G19*14+14+1)+28)-1)</f>
         <v>29|28</v>
       </c>
@@ -3266,7 +3257,7 @@
         <f>_xlfn.CONCAT((I19*14+14+1),"|",(I19*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="I20" s="39" t="str">
+      <c r="I20" s="18" t="str">
         <f>_xlfn.CONCAT(($B$7-(I19*14+14+1)+28), "|", ($B$7-(I19*14+14+1)+28)-1)</f>
         <v>43|42</v>
       </c>
@@ -3274,7 +3265,7 @@
         <f>_xlfn.CONCAT((K19*14+(14*2)+1),"|",(K19*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="K20" s="40" t="str">
+      <c r="K20" s="10" t="str">
         <f>_xlfn.CONCAT(($B$7-(K19*14+1)),"|",($B$7-(K19*14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3282,7 +3273,7 @@
         <f>_xlfn.CONCAT((M19*14+14+1),"|",(M19*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="M20" s="39" t="str">
+      <c r="M20" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(M19*14+14+1)+28), "|", ($B$8-(M19*14+14+1)+28)-1)</f>
         <v>57|56</v>
       </c>
@@ -3290,7 +3281,7 @@
         <f>_xlfn.CONCAT((O19*14+(14*2)+1),"|",(O19*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="O20" s="39" t="str">
+      <c r="O20" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(O19*14+1)),"|",($B$8-(O19*14+1)-1))</f>
         <v>43|42</v>
       </c>
@@ -3298,7 +3289,7 @@
         <f>_xlfn.CONCAT((Q19*14+(14*3)+1),"|",(Q19*14+(14*3)))</f>
         <v>43|42</v>
       </c>
-      <c r="Q20" s="41" t="str">
+      <c r="Q20" s="21" t="str">
         <f>_xlfn.CONCAT(($B$8-(Q19*14+14+1)),"|",($B$8-(Q19*14+14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3356,7 +3347,7 @@
         <f>_xlfn.CONCAT((G21*14+14+1),"|",(G21*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="G22" s="39" t="str">
+      <c r="G22" s="18" t="str">
         <f>_xlfn.CONCAT(($B$6-(G21*14+14+1)+28), "|", ($B$6-(G21*14+14+1)+28)-1)</f>
         <v>29|28</v>
       </c>
@@ -3364,7 +3355,7 @@
         <f>_xlfn.CONCAT((I21*14+14+1),"|",(I21*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="I22" s="39" t="str">
+      <c r="I22" s="18" t="str">
         <f>_xlfn.CONCAT(($B$7-(I21*14+14+1)+28), "|", ($B$7-(I21*14+14+1)+28)-1)</f>
         <v>43|42</v>
       </c>
@@ -3372,7 +3363,7 @@
         <f>_xlfn.CONCAT((K21*14+(14*2)+1),"|",(K21*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="K22" s="40" t="str">
+      <c r="K22" s="10" t="str">
         <f>_xlfn.CONCAT(($B$7-(K21*14+1)),"|",($B$7-(K21*14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3380,7 +3371,7 @@
         <f>_xlfn.CONCAT((M21*14+14+1),"|",(M21*14+14))</f>
         <v>15|14</v>
       </c>
-      <c r="M22" s="39" t="str">
+      <c r="M22" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(M21*14+14+1)+28), "|", ($B$8-(M21*14+14+1)+28)-1)</f>
         <v>57|56</v>
       </c>
@@ -3388,7 +3379,7 @@
         <f>_xlfn.CONCAT((O21*14+(14*2)+1),"|",(O21*14+(14*2)))</f>
         <v>29|28</v>
       </c>
-      <c r="O22" s="39" t="str">
+      <c r="O22" s="18" t="str">
         <f>_xlfn.CONCAT(($B$8-(O21*14+1)),"|",($B$8-(O21*14+1)-1))</f>
         <v>43|42</v>
       </c>
@@ -3396,7 +3387,7 @@
         <f>_xlfn.CONCAT((Q21*14+(14*3)+1),"|",(Q21*14+(14*3)))</f>
         <v>43|42</v>
       </c>
-      <c r="Q22" s="41" t="str">
+      <c r="Q22" s="21" t="str">
         <f>_xlfn.CONCAT(($B$8-(Q21*14+14+1)),"|",($B$8-(Q21*14+14+1)-1))</f>
         <v>29|28</v>
       </c>
@@ -3519,40 +3510,40 @@
       </c>
     </row>
     <row r="34" spans="6:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="52" t="s">
+      <c r="F34" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
     </row>
     <row r="35" spans="6:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F35" s="52" t="s">
+      <c r="F35" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52" t="s">
+      <c r="G35" s="49"/>
+      <c r="H35" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52" t="s">
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
     </row>
     <row r="36" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F36" s="35" t="e" cm="1">
@@ -3929,107 +3920,107 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="expression" dxfId="0" priority="34">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>COUNTIF($I$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18">
-    <cfRule type="expression" dxfId="20" priority="32">
+    <cfRule type="expression" dxfId="19" priority="32">
       <formula>COUNTIF($K$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="expression" dxfId="19" priority="31">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>COUNTIF($K$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="expression" dxfId="18" priority="30">
+    <cfRule type="expression" dxfId="17" priority="30">
       <formula>COUNTIF($K$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:M16">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>COUNTIF($M$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:O16">
-    <cfRule type="expression" dxfId="16" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>COUNTIF($O$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:Q16">
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>COUNTIF($Q$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:M18">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>COUNTIF($M$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:O18">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>COUNTIF($O$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>COUNTIF($Q$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:M20">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>COUNTIF($M$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:O20">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>COUNTIF($O$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:Q20">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>COUNTIF($Q$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:M22">
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>COUNTIF($M$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:O22">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>COUNTIF($O$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:Q22">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>COUNTIF($Q$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:G18">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>COUNTIF($G$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:G20">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>COUNTIF($G$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:G22">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>COUNTIF($G$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:I16">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>COUNTIF($I$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF($K$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4068,27 +4059,27 @@
       <c r="A1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="63"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Adding DMDS double-bond position identification
</commit_message>
<xml_diff>
--- a/CHC-indentification.xlsx
+++ b/CHC-indentification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Trabajo\Proyectos\Chemical Ecology\CHC-identification_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80038E6-A19A-4942-93F3-1AFAC2A6CC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1C399-8DE4-4342-B08C-6478E4D0FE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
   </bookViews>
   <sheets>
     <sheet name="CHC-Identification" sheetId="1" r:id="rId1"/>
@@ -818,8 +818,57 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Daniel Rodriguez Leon</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5DB7C71F-74A1-4769-B493-011E979CE6AD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="10"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The target compound is the compound you are aiming to identify</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{B6AE3FCA-EC55-414B-AFDE-E31D15E24A1C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="10"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Below it is shown the total mass diagnostic ion for your target compound, depending on the expected hydrocarbon class.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -841,7 +890,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="28">
   <si>
     <t>Alkane</t>
   </si>
@@ -902,12 +951,36 @@
   <si>
     <t>The blue fields correspond to the input fields. There you can enter the number corresponding to the expected trait of the hydrocarbon you are aiming to find. The input font color is red.                                                                                                                                                                                                                                                                                                                                                      Yellow cells display information, according to the entry you give to the input fields. These cells change to dark purple to indicate that they are not showing information regarding your target compound.                                                                                                                                                                                                                                                                                                                                                                           Extra explanatory information is displayed when you hover with the mouse over some cells.</t>
   </si>
+  <si>
+    <t>Alkadiene - ring</t>
+  </si>
+  <si>
+    <t>Alkadiene - no-ring</t>
+  </si>
+  <si>
+    <t>A+ (1)</t>
+  </si>
+  <si>
+    <t>A+ (2)</t>
+  </si>
+  <si>
+    <t>Total mass diagnostic Ion (M+) post-DMDS</t>
+  </si>
+  <si>
+    <t>C-chain length</t>
+  </si>
+  <si>
+    <t>A+ (-1)</t>
+  </si>
+  <si>
+    <t>A+ (-2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,6 +1063,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1029,7 +1130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1480,12 +1581,387 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1664,13 +2140,208 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6600CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2039,6 +2710,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3A1953"/>
       <color rgb="FF6600CC"/>
       <color rgb="FFD1B1D7"/>
       <color rgb="FFA8A2D6"/>
@@ -2455,7 +3127,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2465,8 +3137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FD13C8-9C57-4E7C-B7EE-A41A7F7BBBB9}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3764,264 +4436,264 @@
     <mergeCell ref="L14:Q14"/>
     <mergeCell ref="F13:Q13"/>
   </mergeCells>
+  <conditionalFormatting sqref="B3:B8">
+    <cfRule type="expression" dxfId="57" priority="108">
+      <formula>COUNTIF($B$1,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C4:C31">
-    <cfRule type="cellIs" dxfId="51" priority="201" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="201" operator="greaterThanOrEqual">
       <formula>$B$3-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D31">
-    <cfRule type="cellIs" dxfId="50" priority="200" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="200" operator="greaterThanOrEqual">
       <formula>$B$4-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E31">
-    <cfRule type="cellIs" dxfId="49" priority="198" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="198" operator="greaterThanOrEqual">
       <formula>$B$5-14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B8">
-    <cfRule type="expression" dxfId="48" priority="108">
-      <formula>COUNTIF($B$1,"")</formula>
+  <conditionalFormatting sqref="F16:G16">
+    <cfRule type="expression" dxfId="53" priority="41">
+      <formula>COUNTIF($G$15,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:G18">
+    <cfRule type="expression" dxfId="52" priority="5">
+      <formula>COUNTIF($G$17,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:G20">
+    <cfRule type="expression" dxfId="51" priority="4">
+      <formula>COUNTIF($G$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:G22">
+    <cfRule type="expression" dxfId="50" priority="3">
+      <formula>COUNTIF($G$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="47" priority="97">
+    <cfRule type="expression" dxfId="49" priority="97">
       <formula>COUNTIF(F$6:G$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="46" priority="90">
-      <formula>COUNTIF(J6:K6,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="45" priority="89">
-      <formula>COUNTIF(L6:M6,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="44" priority="88">
-      <formula>COUNTIF(N6:O6,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="43" priority="87">
-      <formula>COUNTIF(P6:Q6,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="42" priority="86">
+    <cfRule type="expression" dxfId="48" priority="86">
       <formula>COUNTIF(F8:G8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="41" priority="68">
+    <cfRule type="expression" dxfId="47" priority="68">
       <formula>COUNTIF(F10:G10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="40" priority="67">
+    <cfRule type="expression" dxfId="46" priority="67">
       <formula>COUNTIF(F12:G12,"")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H16:I16">
+    <cfRule type="expression" dxfId="45" priority="2">
+      <formula>COUNTIF($I$15,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:I18">
+    <cfRule type="expression" dxfId="44" priority="36">
+      <formula>COUNTIF($I$17,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:I20">
+    <cfRule type="expression" dxfId="43" priority="35">
+      <formula>COUNTIF($I$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:I22">
+    <cfRule type="expression" dxfId="42" priority="34">
+      <formula>COUNTIF($I$21,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="39" priority="65">
+    <cfRule type="expression" dxfId="41" priority="65">
       <formula>COUNTIF(H$6:I$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="38" priority="60">
+    <cfRule type="expression" dxfId="40" priority="60">
       <formula>COUNTIF(H8:I8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="37" priority="57">
+    <cfRule type="expression" dxfId="39" priority="57">
       <formula>COUNTIF(H10:I10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="36" priority="56">
+    <cfRule type="expression" dxfId="38" priority="56">
       <formula>COUNTIF(H12:I12,"")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J16:K16">
+    <cfRule type="expression" dxfId="37" priority="1">
+      <formula>COUNTIF($K$15,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:K18">
+    <cfRule type="expression" dxfId="36" priority="32">
+      <formula>COUNTIF($K$17,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:K20">
+    <cfRule type="expression" dxfId="35" priority="31">
+      <formula>COUNTIF($K$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22:K22">
+    <cfRule type="expression" dxfId="34" priority="30">
+      <formula>COUNTIF($K$21,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="expression" dxfId="33" priority="90">
+      <formula>COUNTIF(J6:K6,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="expression" dxfId="32" priority="52">
+      <formula>COUNTIF(J8:K8,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="35" priority="54">
+    <cfRule type="expression" dxfId="31" priority="54">
       <formula>COUNTIF(J10:K10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="34" priority="53">
+    <cfRule type="expression" dxfId="30" priority="53">
       <formula>COUNTIF(J12:K12,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="33" priority="52">
-      <formula>COUNTIF(J8:K8,"")</formula>
+  <conditionalFormatting sqref="L16:M16">
+    <cfRule type="expression" dxfId="29" priority="17">
+      <formula>COUNTIF($M$15,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18:M18">
+    <cfRule type="expression" dxfId="28" priority="14">
+      <formula>COUNTIF($M$17,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L20:M20">
+    <cfRule type="expression" dxfId="27" priority="13">
+      <formula>COUNTIF($M$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22:M22">
+    <cfRule type="expression" dxfId="26" priority="12">
+      <formula>COUNTIF($M$21,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5">
+    <cfRule type="expression" dxfId="25" priority="89">
+      <formula>COUNTIF(L6:M6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="32" priority="50">
+    <cfRule type="expression" dxfId="24" priority="50">
       <formula>COUNTIF(L8:M8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="expression" dxfId="31" priority="49">
+    <cfRule type="expression" dxfId="23" priority="49">
       <formula>COUNTIF(L10:M10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="30" priority="48">
+    <cfRule type="expression" dxfId="22" priority="48">
       <formula>COUNTIF(L12:M12,"")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N16:O16">
+    <cfRule type="expression" dxfId="21" priority="16">
+      <formula>COUNTIF($O$15,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18:O18">
+    <cfRule type="expression" dxfId="20" priority="11">
+      <formula>COUNTIF($O$17,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N20:O20">
+    <cfRule type="expression" dxfId="19" priority="10">
+      <formula>COUNTIF($O$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N22:O22">
+    <cfRule type="expression" dxfId="18" priority="9">
+      <formula>COUNTIF($O$21,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="expression" dxfId="17" priority="88">
+      <formula>COUNTIF(N6:O6,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="29" priority="47">
+    <cfRule type="expression" dxfId="16" priority="47">
       <formula>COUNTIF(N8:O8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="28" priority="46">
+    <cfRule type="expression" dxfId="15" priority="46">
       <formula>COUNTIF(N10:O10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="expression" dxfId="27" priority="45">
+    <cfRule type="expression" dxfId="14" priority="45">
       <formula>COUNTIF(N12:O12,"")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P16:Q16">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>COUNTIF($Q$15,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18:Q18">
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>COUNTIF($Q$17,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P20:Q20">
+    <cfRule type="expression" dxfId="11" priority="7">
+      <formula>COUNTIF($Q$19,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P22:Q22">
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>COUNTIF($Q$21,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5">
+    <cfRule type="expression" dxfId="9" priority="87">
+      <formula>COUNTIF(P6:Q6,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="expression" dxfId="26" priority="44">
+    <cfRule type="expression" dxfId="8" priority="44">
       <formula>COUNTIF(P8:Q8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9">
-    <cfRule type="expression" dxfId="25" priority="43">
+    <cfRule type="expression" dxfId="7" priority="43">
       <formula>COUNTIF(P10:Q10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="expression" dxfId="24" priority="42">
+    <cfRule type="expression" dxfId="6" priority="42">
       <formula>COUNTIF(P12:Q12,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16:G16">
-    <cfRule type="expression" dxfId="23" priority="41">
-      <formula>COUNTIF($G$15,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18:I18">
-    <cfRule type="expression" dxfId="22" priority="36">
-      <formula>COUNTIF($I$17,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:I20">
-    <cfRule type="expression" dxfId="21" priority="35">
-      <formula>COUNTIF($I$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22:I22">
-    <cfRule type="expression" dxfId="20" priority="34">
-      <formula>COUNTIF($I$21,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18:K18">
-    <cfRule type="expression" dxfId="19" priority="32">
-      <formula>COUNTIF($K$17,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J20:K20">
-    <cfRule type="expression" dxfId="18" priority="31">
-      <formula>COUNTIF($K$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22:K22">
-    <cfRule type="expression" dxfId="17" priority="30">
-      <formula>COUNTIF($K$21,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L16:M16">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>COUNTIF($M$15,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N16:O16">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>COUNTIF($O$15,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P16:Q16">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>COUNTIF($Q$15,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L18:M18">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>COUNTIF($M$17,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N18:O18">
-    <cfRule type="expression" dxfId="12" priority="11">
-      <formula>COUNTIF($O$17,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="11" priority="8">
-      <formula>COUNTIF($Q$17,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L20:M20">
-    <cfRule type="expression" dxfId="10" priority="13">
-      <formula>COUNTIF($M$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N20:O20">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>COUNTIF($O$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P20:Q20">
-    <cfRule type="expression" dxfId="8" priority="7">
-      <formula>COUNTIF($Q$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L22:M22">
-    <cfRule type="expression" dxfId="7" priority="12">
-      <formula>COUNTIF($M$21,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22:O22">
-    <cfRule type="expression" dxfId="6" priority="9">
-      <formula>COUNTIF($O$21,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P22:Q22">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>COUNTIF($Q$21,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18:G18">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>COUNTIF($G$17,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20:G20">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>COUNTIF($G$19,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22:G22">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>COUNTIF($G$21,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:I16">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>COUNTIF($I$15,"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16:K16">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($K$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
@@ -4094,15 +4766,977 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A751E-AC0F-4038-95D2-ABBAAB30BEF5}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A751E-AC0F-4038-95D2-ABBAAB30BEF5}">
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="17.7109375" style="64" customWidth="1"/>
+    <col min="10" max="13" width="1.5703125" style="64" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125" style="64" customWidth="1"/>
+    <col min="16" max="16384" width="10.140625" style="64"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="61" customFormat="1" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="82"/>
+    </row>
+    <row r="2" spans="1:15" s="61" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="97"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
+    </row>
+    <row r="3" spans="1:15" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="76"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="66">
+        <f>B2*14+94</f>
+        <v>94</v>
+      </c>
+      <c r="E3" s="108"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+    </row>
+    <row r="4" spans="1:15" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="76"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="66"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="107"/>
+      <c r="O4" s="107"/>
+    </row>
+    <row r="5" spans="1:15" s="61" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="78"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="107"/>
+    </row>
+    <row r="6" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="80"/>
+      <c r="D6" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="98"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="98"/>
+      <c r="I6" s="63"/>
+    </row>
+    <row r="7" spans="1:15" s="94" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="90"/>
+      <c r="B7" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="103" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="87" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="95">
+        <v>1</v>
+      </c>
+      <c r="B8" s="104">
+        <v>61</v>
+      </c>
+      <c r="C8" s="88"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="91">
+        <v>2</v>
+      </c>
+      <c r="B9" s="105">
+        <f>B$8+(14*A8)</f>
+        <v>75</v>
+      </c>
+      <c r="C9" s="70">
+        <f>(($B$2-1)*14)+$B$8</f>
+        <v>47</v>
+      </c>
+      <c r="D9" s="99"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="70"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="91">
+        <v>3</v>
+      </c>
+      <c r="B10" s="105">
+        <f>B$8+(14*A9)</f>
+        <v>89</v>
+      </c>
+      <c r="C10" s="70">
+        <f t="shared" ref="C10:C46" si="0">(($B$2-1)*14)+$B$8</f>
+        <v>47</v>
+      </c>
+      <c r="D10" s="99"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="70"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="91">
+        <v>4</v>
+      </c>
+      <c r="B11" s="105">
+        <f>B$8+(14*A10)</f>
+        <v>103</v>
+      </c>
+      <c r="C11" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D11" s="99"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="70"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="91">
+        <v>5</v>
+      </c>
+      <c r="B12" s="105">
+        <f>B$8+(14*A11)</f>
+        <v>117</v>
+      </c>
+      <c r="C12" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D12" s="99"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="70"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="91">
+        <v>6</v>
+      </c>
+      <c r="B13" s="105">
+        <f>B$8+(14*A12)</f>
+        <v>131</v>
+      </c>
+      <c r="C13" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D13" s="99"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="70"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="91">
+        <v>7</v>
+      </c>
+      <c r="B14" s="105">
+        <f>B$8+(14*A13)</f>
+        <v>145</v>
+      </c>
+      <c r="C14" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D14" s="99"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="70"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="91">
+        <v>8</v>
+      </c>
+      <c r="B15" s="105">
+        <f>B$8+(14*A14)</f>
+        <v>159</v>
+      </c>
+      <c r="C15" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D15" s="99"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="70"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="91">
+        <v>9</v>
+      </c>
+      <c r="B16" s="105">
+        <f>B$8+(14*A15)</f>
+        <v>173</v>
+      </c>
+      <c r="C16" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D16" s="99"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="99"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="91">
+        <v>10</v>
+      </c>
+      <c r="B17" s="105">
+        <f>B$8+(14*A16)</f>
+        <v>187</v>
+      </c>
+      <c r="C17" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D17" s="99"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="70"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="91">
+        <v>11</v>
+      </c>
+      <c r="B18" s="105">
+        <f>B$8+(14*A17)</f>
+        <v>201</v>
+      </c>
+      <c r="C18" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D18" s="99"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="91">
+        <v>12</v>
+      </c>
+      <c r="B19" s="105">
+        <f>B$8+(14*A18)</f>
+        <v>215</v>
+      </c>
+      <c r="C19" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D19" s="99"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="70"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="91">
+        <v>13</v>
+      </c>
+      <c r="B20" s="105">
+        <f>B$8+(14*A19)</f>
+        <v>229</v>
+      </c>
+      <c r="C20" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D20" s="99"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="70"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="91">
+        <v>14</v>
+      </c>
+      <c r="B21" s="105">
+        <f>B$8+(14*A20)</f>
+        <v>243</v>
+      </c>
+      <c r="C21" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D21" s="99"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="70"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="91">
+        <v>15</v>
+      </c>
+      <c r="B22" s="105">
+        <f>B$8+(14*A21)</f>
+        <v>257</v>
+      </c>
+      <c r="C22" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D22" s="99"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="70"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="91">
+        <v>16</v>
+      </c>
+      <c r="B23" s="105">
+        <f>B$8+(14*A22)</f>
+        <v>271</v>
+      </c>
+      <c r="C23" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D23" s="99"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="70"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="91">
+        <v>17</v>
+      </c>
+      <c r="B24" s="105">
+        <f>B$8+(14*A23)</f>
+        <v>285</v>
+      </c>
+      <c r="C24" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D24" s="99"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="70"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="91">
+        <v>18</v>
+      </c>
+      <c r="B25" s="105">
+        <f>B$8+(14*A24)</f>
+        <v>299</v>
+      </c>
+      <c r="C25" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D25" s="99"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="70"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="91">
+        <v>19</v>
+      </c>
+      <c r="B26" s="105">
+        <f>B$8+(14*A25)</f>
+        <v>313</v>
+      </c>
+      <c r="C26" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D26" s="99"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="99"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="70"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="91">
+        <v>20</v>
+      </c>
+      <c r="B27" s="105">
+        <f>B$8+(14*A26)</f>
+        <v>327</v>
+      </c>
+      <c r="C27" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D27" s="99"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="70"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="91">
+        <v>21</v>
+      </c>
+      <c r="B28" s="105">
+        <f>B$8+(14*A27)</f>
+        <v>341</v>
+      </c>
+      <c r="C28" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D28" s="99"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="70"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="91">
+        <v>22</v>
+      </c>
+      <c r="B29" s="105">
+        <f>B$8+(14*A28)</f>
+        <v>355</v>
+      </c>
+      <c r="C29" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D29" s="99"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="99"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="70"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="91">
+        <v>23</v>
+      </c>
+      <c r="B30" s="105">
+        <f>B$8+(14*A29)</f>
+        <v>369</v>
+      </c>
+      <c r="C30" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D30" s="99"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="99"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="70"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="91">
+        <v>24</v>
+      </c>
+      <c r="B31" s="105">
+        <f>B$8+(14*A30)</f>
+        <v>383</v>
+      </c>
+      <c r="C31" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D31" s="99"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="70"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="91">
+        <v>25</v>
+      </c>
+      <c r="B32" s="105">
+        <f>B$8+(14*A31)</f>
+        <v>397</v>
+      </c>
+      <c r="C32" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D32" s="99"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="99"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="70"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="91">
+        <v>26</v>
+      </c>
+      <c r="B33" s="105">
+        <f>B$8+(14*A32)</f>
+        <v>411</v>
+      </c>
+      <c r="C33" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D33" s="99"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="99"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="91">
+        <v>27</v>
+      </c>
+      <c r="B34" s="105">
+        <f>B$8+(14*A33)</f>
+        <v>425</v>
+      </c>
+      <c r="C34" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D34" s="99"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="91">
+        <v>28</v>
+      </c>
+      <c r="B35" s="105">
+        <f>B$8+(14*A34)</f>
+        <v>439</v>
+      </c>
+      <c r="C35" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D35" s="99"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="70"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="91">
+        <v>29</v>
+      </c>
+      <c r="B36" s="105">
+        <f>B$8+(14*A35)</f>
+        <v>453</v>
+      </c>
+      <c r="C36" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D36" s="99"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="91">
+        <v>30</v>
+      </c>
+      <c r="B37" s="105">
+        <f>B$8+(14*A36)</f>
+        <v>467</v>
+      </c>
+      <c r="C37" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D37" s="99"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="99"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="70"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="91">
+        <v>31</v>
+      </c>
+      <c r="B38" s="105">
+        <f>B$8+(14*A37)</f>
+        <v>481</v>
+      </c>
+      <c r="C38" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D38" s="99"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="70"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="91">
+        <v>32</v>
+      </c>
+      <c r="B39" s="105">
+        <f>B$8+(14*A38)</f>
+        <v>495</v>
+      </c>
+      <c r="C39" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D39" s="99"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="70"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="91">
+        <v>33</v>
+      </c>
+      <c r="B40" s="105">
+        <f>B$8+(14*A39)</f>
+        <v>509</v>
+      </c>
+      <c r="C40" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D40" s="99"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="99"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="70"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="91">
+        <v>34</v>
+      </c>
+      <c r="B41" s="105">
+        <f>B$8+(14*A40)</f>
+        <v>523</v>
+      </c>
+      <c r="C41" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D41" s="99"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="99"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="70"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="91">
+        <v>35</v>
+      </c>
+      <c r="B42" s="105">
+        <f>B$8+(14*A41)</f>
+        <v>537</v>
+      </c>
+      <c r="C42" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D42" s="99"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="99"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="70"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="91">
+        <v>36</v>
+      </c>
+      <c r="B43" s="105">
+        <f>B$8+(14*A42)</f>
+        <v>551</v>
+      </c>
+      <c r="C43" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D43" s="99"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="99"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="70"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="91">
+        <v>37</v>
+      </c>
+      <c r="B44" s="105">
+        <f>B$8+(14*A43)</f>
+        <v>565</v>
+      </c>
+      <c r="C44" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D44" s="99"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="99"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="70"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="91">
+        <v>38</v>
+      </c>
+      <c r="B45" s="105">
+        <f>B$8+(14*A44)</f>
+        <v>579</v>
+      </c>
+      <c r="C45" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D45" s="99"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="99"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="70"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="91">
+        <v>39</v>
+      </c>
+      <c r="B46" s="105">
+        <f>B$8+(14*A45)</f>
+        <v>593</v>
+      </c>
+      <c r="C46" s="70">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D46" s="99"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="99"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="70"/>
+    </row>
+    <row r="47" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="92">
+        <v>40</v>
+      </c>
+      <c r="B47" s="106">
+        <f>B$8+(14*A46)</f>
+        <v>607</v>
+      </c>
+      <c r="C47" s="72">
+        <f>(($B$2-1)*14)+$B$8</f>
+        <v>47</v>
+      </c>
+      <c r="D47" s="100"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="100"/>
+      <c r="H47" s="71"/>
+      <c r="I47" s="72"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E2:I5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D3:D5">
+    <cfRule type="expression" dxfId="5" priority="11">
+      <formula>COUNTIF($B$2,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G47 B8:D47">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+      <formula>$B$8+(($B$2-1)*14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:H47">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+      <formula>$B$8+(($B$2-1)*14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:I47">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>$B$8+(($B$2-1)*14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:F47">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>$B$8+(($B$2-1)*14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C47">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>B9&gt;C9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydrocarbon chain length" prompt="Enter a whole number (greater than 1) indicating the number of carbons in the hydrocarbon chain of your target compound." sqref="B2" xr:uid="{F7014332-3719-4885-95BF-44AFD9FD41C8}">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Information display cell" prompt="Do not modify the content of this cell!_x000a_" sqref="D3:D5" xr:uid="{21ECB7F2-771B-4437-8B65-3F0ADFF96332}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Setting to start at the first page
</commit_message>
<xml_diff>
--- a/CHC-indentification.xlsx
+++ b/CHC-indentification.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Trabajo\Proyectos\Chemical Ecology\CHC-identification_tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CHC-identification_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1C399-8DE4-4342-B08C-6478E4D0FE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD46C0D9-1FB6-4968-8600-D7C5639F5AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
   </bookViews>
   <sheets>
     <sheet name="CHC-Identification" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -890,7 +890,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
   <si>
     <t>Alkane</t>
   </si>
@@ -958,22 +958,19 @@
     <t>Alkadiene - no-ring</t>
   </si>
   <si>
-    <t>A+ (1)</t>
-  </si>
-  <si>
-    <t>A+ (2)</t>
-  </si>
-  <si>
     <t>Total mass diagnostic Ion (M+) post-DMDS</t>
   </si>
   <si>
     <t>C-chain length</t>
   </si>
   <si>
-    <t>A+ (-1)</t>
+    <t>A+ (a)</t>
   </si>
   <si>
-    <t>A+ (-2)</t>
+    <t>A+ (b)</t>
+  </si>
+  <si>
+    <t>A+ (-b)</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1597,21 +1594,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1711,7 +1693,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -1721,35 +1703,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -1846,26 +1800,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1940,17 +1874,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1961,7 +1884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2075,6 +1998,81 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2141,109 +2139,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2252,54 +2148,60 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="56">
     <dxf>
       <fill>
         <patternFill>
@@ -2325,20 +2227,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3137,7 +3025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FD13C8-9C57-4E7C-B7EE-A41A7F7BBBB9}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3154,47 +3042,47 @@
         <v>3</v>
       </c>
       <c r="B1" s="24"/>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="47" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="48"/>
+      <c r="P1" s="73"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="65"/>
+      <c r="C2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="71"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3213,20 +3101,20 @@
       <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="52"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="77"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -3247,24 +3135,24 @@
         <f>D4-2</f>
         <v>39</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54" t="s">
+      <c r="G4" s="79"/>
+      <c r="H4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56" t="s">
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="58"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="83"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -3626,20 +3514,20 @@
         <f t="shared" si="8"/>
         <v>165</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="52"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="76"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="76"/>
+      <c r="Q13" s="77"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="11">
@@ -3653,24 +3541,24 @@
         <f t="shared" si="9"/>
         <v>179</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54" t="s">
+      <c r="G14" s="79"/>
+      <c r="H14" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="56" t="s">
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="58"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="83"/>
     </row>
     <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="C15" s="11">
@@ -4182,40 +4070,40 @@
       </c>
     </row>
     <row r="34" spans="6:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="49" t="s">
+      <c r="F34" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="49"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="74"/>
+      <c r="O34" s="74"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="74"/>
     </row>
     <row r="35" spans="6:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F35" s="49" t="s">
+      <c r="F35" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49" t="s">
+      <c r="G35" s="74"/>
+      <c r="H35" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49" t="s">
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="49"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="74"/>
+      <c r="O35" s="74"/>
+      <c r="P35" s="74"/>
+      <c r="Q35" s="74"/>
     </row>
     <row r="36" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F36" s="35" t="e" cm="1">
@@ -4437,262 +4325,262 @@
     <mergeCell ref="F13:Q13"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="expression" dxfId="57" priority="108">
+    <cfRule type="expression" dxfId="55" priority="108">
       <formula>COUNTIF($B$1,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C31">
-    <cfRule type="cellIs" dxfId="56" priority="201" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="201" operator="greaterThanOrEqual">
       <formula>$B$3-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D31">
-    <cfRule type="cellIs" dxfId="55" priority="200" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="200" operator="greaterThanOrEqual">
       <formula>$B$4-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E31">
-    <cfRule type="cellIs" dxfId="54" priority="198" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="198" operator="greaterThanOrEqual">
       <formula>$B$5-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16">
-    <cfRule type="expression" dxfId="53" priority="41">
+    <cfRule type="expression" dxfId="51" priority="41">
       <formula>COUNTIF($G$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:G18">
-    <cfRule type="expression" dxfId="52" priority="5">
+    <cfRule type="expression" dxfId="50" priority="5">
       <formula>COUNTIF($G$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:G20">
-    <cfRule type="expression" dxfId="51" priority="4">
+    <cfRule type="expression" dxfId="49" priority="4">
       <formula>COUNTIF($G$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:G22">
-    <cfRule type="expression" dxfId="50" priority="3">
+    <cfRule type="expression" dxfId="48" priority="3">
       <formula>COUNTIF($G$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="49" priority="97">
+    <cfRule type="expression" dxfId="47" priority="97">
       <formula>COUNTIF(F$6:G$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="48" priority="86">
+    <cfRule type="expression" dxfId="46" priority="86">
       <formula>COUNTIF(F8:G8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="47" priority="68">
+    <cfRule type="expression" dxfId="45" priority="68">
       <formula>COUNTIF(F10:G10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="46" priority="67">
+    <cfRule type="expression" dxfId="44" priority="67">
       <formula>COUNTIF(F12:G12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:I16">
-    <cfRule type="expression" dxfId="45" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>COUNTIF($I$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:I18">
-    <cfRule type="expression" dxfId="44" priority="36">
+    <cfRule type="expression" dxfId="42" priority="36">
       <formula>COUNTIF($I$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:I20">
-    <cfRule type="expression" dxfId="43" priority="35">
+    <cfRule type="expression" dxfId="41" priority="35">
       <formula>COUNTIF($I$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="expression" dxfId="42" priority="34">
+    <cfRule type="expression" dxfId="40" priority="34">
       <formula>COUNTIF($I$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="41" priority="65">
+    <cfRule type="expression" dxfId="39" priority="65">
       <formula>COUNTIF(H$6:I$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="40" priority="60">
+    <cfRule type="expression" dxfId="38" priority="60">
       <formula>COUNTIF(H8:I8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="39" priority="57">
+    <cfRule type="expression" dxfId="37" priority="57">
       <formula>COUNTIF(H10:I10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="38" priority="56">
+    <cfRule type="expression" dxfId="36" priority="56">
       <formula>COUNTIF(H12:I12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16">
-    <cfRule type="expression" dxfId="37" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>COUNTIF($K$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18">
-    <cfRule type="expression" dxfId="36" priority="32">
+    <cfRule type="expression" dxfId="34" priority="32">
       <formula>COUNTIF($K$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="expression" dxfId="35" priority="31">
+    <cfRule type="expression" dxfId="33" priority="31">
       <formula>COUNTIF($K$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="expression" dxfId="34" priority="30">
+    <cfRule type="expression" dxfId="32" priority="30">
       <formula>COUNTIF($K$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="33" priority="90">
+    <cfRule type="expression" dxfId="31" priority="90">
       <formula>COUNTIF(J6:K6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="32" priority="52">
+    <cfRule type="expression" dxfId="30" priority="52">
       <formula>COUNTIF(J8:K8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="31" priority="54">
+    <cfRule type="expression" dxfId="29" priority="54">
       <formula>COUNTIF(J10:K10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="30" priority="53">
+    <cfRule type="expression" dxfId="28" priority="53">
       <formula>COUNTIF(J12:K12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:M16">
-    <cfRule type="expression" dxfId="29" priority="17">
+    <cfRule type="expression" dxfId="27" priority="17">
       <formula>COUNTIF($M$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:M18">
-    <cfRule type="expression" dxfId="28" priority="14">
+    <cfRule type="expression" dxfId="26" priority="14">
       <formula>COUNTIF($M$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:M20">
-    <cfRule type="expression" dxfId="27" priority="13">
+    <cfRule type="expression" dxfId="25" priority="13">
       <formula>COUNTIF($M$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:M22">
-    <cfRule type="expression" dxfId="26" priority="12">
+    <cfRule type="expression" dxfId="24" priority="12">
       <formula>COUNTIF($M$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="25" priority="89">
+    <cfRule type="expression" dxfId="23" priority="89">
       <formula>COUNTIF(L6:M6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="24" priority="50">
+    <cfRule type="expression" dxfId="22" priority="50">
       <formula>COUNTIF(L8:M8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="expression" dxfId="23" priority="49">
+    <cfRule type="expression" dxfId="21" priority="49">
       <formula>COUNTIF(L10:M10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="22" priority="48">
+    <cfRule type="expression" dxfId="20" priority="48">
       <formula>COUNTIF(L12:M12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:O16">
-    <cfRule type="expression" dxfId="21" priority="16">
+    <cfRule type="expression" dxfId="19" priority="16">
       <formula>COUNTIF($O$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:O18">
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>COUNTIF($O$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:O20">
-    <cfRule type="expression" dxfId="19" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>COUNTIF($O$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:O22">
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>COUNTIF($O$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="17" priority="88">
+    <cfRule type="expression" dxfId="15" priority="88">
       <formula>COUNTIF(N6:O6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="16" priority="47">
+    <cfRule type="expression" dxfId="14" priority="47">
       <formula>COUNTIF(N8:O8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="15" priority="46">
+    <cfRule type="expression" dxfId="13" priority="46">
       <formula>COUNTIF(N10:O10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="expression" dxfId="14" priority="45">
+    <cfRule type="expression" dxfId="12" priority="45">
       <formula>COUNTIF(N12:O12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:Q16">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>COUNTIF($Q$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>COUNTIF($Q$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:Q20">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>COUNTIF($Q$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:Q22">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>COUNTIF($Q$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="9" priority="87">
+    <cfRule type="expression" dxfId="7" priority="87">
       <formula>COUNTIF(P6:Q6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="expression" dxfId="8" priority="44">
+    <cfRule type="expression" dxfId="6" priority="44">
       <formula>COUNTIF(P8:Q8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9">
-    <cfRule type="expression" dxfId="7" priority="43">
+    <cfRule type="expression" dxfId="5" priority="43">
       <formula>COUNTIF(P10:Q10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="expression" dxfId="6" priority="42">
+    <cfRule type="expression" dxfId="4" priority="42">
       <formula>COUNTIF(P12:Q12,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4731,27 +4619,27 @@
       <c r="A1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="60"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4767,966 +4655,934 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A751E-AC0F-4038-95D2-ABBAAB30BEF5}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="17.7109375" style="64" customWidth="1"/>
-    <col min="10" max="13" width="1.5703125" style="64" customWidth="1"/>
-    <col min="14" max="15" width="10.5703125" style="64" customWidth="1"/>
-    <col min="16" max="16384" width="10.140625" style="64"/>
+    <col min="1" max="6" width="17.7109375" style="41" customWidth="1"/>
+    <col min="7" max="10" width="1.5703125" style="41" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" style="41" customWidth="1"/>
+    <col min="13" max="16384" width="10.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="61" customFormat="1" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:12" s="39" customFormat="1" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="82" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="82"/>
-    </row>
-    <row r="2" spans="1:15" s="61" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="L1" s="86"/>
+    </row>
+    <row r="2" spans="1:12" s="39" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="96" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-    </row>
-    <row r="3" spans="1:15" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="65" t="s">
+      <c r="B2" s="99"/>
+      <c r="C2" s="87" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="88"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+    </row>
+    <row r="3" spans="1:12" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="103"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="66">
+      <c r="D3" s="43">
         <f>B2*14+94</f>
         <v>94</v>
       </c>
-      <c r="E3" s="108"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-    </row>
-    <row r="4" spans="1:15" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="65" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+    </row>
+    <row r="4" spans="1:12" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="103"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="107"/>
-    </row>
-    <row r="5" spans="1:15" s="61" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="67" t="s">
+      <c r="D4" s="43">
+        <f>D3+92</f>
+        <v>186</v>
+      </c>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+    </row>
+    <row r="5" spans="1:12" s="39" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="104"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
-    </row>
-    <row r="6" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="45"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+    </row>
+    <row r="6" spans="1:12" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="96"/>
+      <c r="D6" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="94"/>
+    </row>
+    <row r="7" spans="1:12" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="90"/>
+      <c r="B7" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="D7" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="51">
         <v>1</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="98"/>
-      <c r="I6" s="63"/>
-    </row>
-    <row r="7" spans="1:15" s="94" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="103" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="87" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="87" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="95">
-        <v>1</v>
-      </c>
-      <c r="B8" s="104">
+      <c r="B8" s="59">
         <v>61</v>
       </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="91">
+      <c r="C8" s="43">
+        <f>$D$3-B8</f>
+        <v>33</v>
+      </c>
+      <c r="D8" s="63">
+        <f>$D$4-B8</f>
+        <v>125</v>
+      </c>
+      <c r="E8" s="57"/>
+      <c r="F8" s="48"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="52">
         <v>2</v>
       </c>
-      <c r="B9" s="105">
+      <c r="B9" s="60">
         <f>B$8+(14*A8)</f>
         <v>75</v>
       </c>
-      <c r="C9" s="70">
-        <f>(($B$2-1)*14)+$B$8</f>
-        <v>47</v>
-      </c>
-      <c r="D9" s="99"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="91">
+      <c r="C9" s="43">
+        <f t="shared" ref="C9:C47" si="0">$D$3-B9</f>
+        <v>19</v>
+      </c>
+      <c r="D9" s="63">
+        <f>$D$4-B9</f>
+        <v>111</v>
+      </c>
+      <c r="E9" s="55"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="52">
         <v>3</v>
       </c>
-      <c r="B10" s="105">
-        <f>B$8+(14*A9)</f>
+      <c r="B10" s="60">
+        <f t="shared" ref="B10:B47" si="1">B$8+(14*A9)</f>
         <v>89</v>
       </c>
-      <c r="C10" s="70">
-        <f t="shared" ref="C10:C46" si="0">(($B$2-1)*14)+$B$8</f>
-        <v>47</v>
-      </c>
-      <c r="D10" s="99"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="91">
+      <c r="C10" s="43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="63">
+        <f t="shared" ref="D10:D47" si="2">$D$4-B10</f>
+        <v>97</v>
+      </c>
+      <c r="E10" s="55"/>
+      <c r="F10" s="46"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="52">
         <v>4</v>
       </c>
-      <c r="B11" s="105">
-        <f>B$8+(14*A10)</f>
+      <c r="B11" s="60">
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="C11" s="70">
+      <c r="C11" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D11" s="99"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="70"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="91">
+        <v>-9</v>
+      </c>
+      <c r="D11" s="63">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="E11" s="55"/>
+      <c r="F11" s="46"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="52">
         <v>5</v>
       </c>
-      <c r="B12" s="105">
-        <f>B$8+(14*A11)</f>
+      <c r="B12" s="60">
+        <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="C12" s="70">
+      <c r="C12" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="70"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="91">
+        <v>-23</v>
+      </c>
+      <c r="D12" s="63">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="E12" s="55"/>
+      <c r="F12" s="46"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="52">
         <v>6</v>
       </c>
-      <c r="B13" s="105">
-        <f>B$8+(14*A12)</f>
+      <c r="B13" s="60">
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
-      <c r="C13" s="70">
+      <c r="C13" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D13" s="99"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="70"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="91">
+        <v>-37</v>
+      </c>
+      <c r="D13" s="63">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="E13" s="55"/>
+      <c r="F13" s="46"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="52">
         <v>7</v>
       </c>
-      <c r="B14" s="105">
-        <f>B$8+(14*A13)</f>
+      <c r="B14" s="60">
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="C14" s="70">
+      <c r="C14" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D14" s="99"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="70"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="91">
+        <v>-51</v>
+      </c>
+      <c r="D14" s="63">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E14" s="55"/>
+      <c r="F14" s="46"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="52">
         <v>8</v>
       </c>
-      <c r="B15" s="105">
-        <f>B$8+(14*A14)</f>
+      <c r="B15" s="60">
+        <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="C15" s="70">
+      <c r="C15" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D15" s="99"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="70"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="91">
+        <v>-65</v>
+      </c>
+      <c r="D15" s="63">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="46"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="52">
         <v>9</v>
       </c>
-      <c r="B16" s="105">
-        <f>B$8+(14*A15)</f>
+      <c r="B16" s="60">
+        <f t="shared" si="1"/>
         <v>173</v>
       </c>
-      <c r="C16" s="70">
+      <c r="C16" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D16" s="99"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="70"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="91">
+        <v>-79</v>
+      </c>
+      <c r="D16" s="63">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="46"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="52">
         <v>10</v>
       </c>
-      <c r="B17" s="105">
-        <f>B$8+(14*A16)</f>
+      <c r="B17" s="60">
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
-      <c r="C17" s="70">
+      <c r="C17" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D17" s="99"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="70"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="91">
+        <v>-93</v>
+      </c>
+      <c r="D17" s="63">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E17" s="55"/>
+      <c r="F17" s="46"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="52">
         <v>11</v>
       </c>
-      <c r="B18" s="105">
-        <f>B$8+(14*A17)</f>
+      <c r="B18" s="60">
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
-      <c r="C18" s="70">
+      <c r="C18" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D18" s="99"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="70"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="91">
+        <v>-107</v>
+      </c>
+      <c r="D18" s="63">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+      <c r="E18" s="55"/>
+      <c r="F18" s="46"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="52">
         <v>12</v>
       </c>
-      <c r="B19" s="105">
-        <f>B$8+(14*A18)</f>
+      <c r="B19" s="60">
+        <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="C19" s="70">
+      <c r="C19" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D19" s="99"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="70"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="91">
+        <v>-121</v>
+      </c>
+      <c r="D19" s="63">
+        <f t="shared" si="2"/>
+        <v>-29</v>
+      </c>
+      <c r="E19" s="55"/>
+      <c r="F19" s="46"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="52">
         <v>13</v>
       </c>
-      <c r="B20" s="105">
-        <f>B$8+(14*A19)</f>
+      <c r="B20" s="60">
+        <f t="shared" si="1"/>
         <v>229</v>
       </c>
-      <c r="C20" s="70">
+      <c r="C20" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D20" s="99"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="70"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="91">
+        <v>-135</v>
+      </c>
+      <c r="D20" s="63">
+        <f t="shared" si="2"/>
+        <v>-43</v>
+      </c>
+      <c r="E20" s="55"/>
+      <c r="F20" s="46"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="52">
         <v>14</v>
       </c>
-      <c r="B21" s="105">
-        <f>B$8+(14*A20)</f>
+      <c r="B21" s="60">
+        <f t="shared" si="1"/>
         <v>243</v>
       </c>
-      <c r="C21" s="70">
+      <c r="C21" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D21" s="99"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="70"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="91">
+        <v>-149</v>
+      </c>
+      <c r="D21" s="63">
+        <f t="shared" si="2"/>
+        <v>-57</v>
+      </c>
+      <c r="E21" s="55"/>
+      <c r="F21" s="46"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="52">
         <v>15</v>
       </c>
-      <c r="B22" s="105">
-        <f>B$8+(14*A21)</f>
+      <c r="B22" s="60">
+        <f t="shared" si="1"/>
         <v>257</v>
       </c>
-      <c r="C22" s="70">
+      <c r="C22" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D22" s="99"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="70"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="91">
+        <v>-163</v>
+      </c>
+      <c r="D22" s="63">
+        <f>$D$4-B22</f>
+        <v>-71</v>
+      </c>
+      <c r="E22" s="55"/>
+      <c r="F22" s="46"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="52">
         <v>16</v>
       </c>
-      <c r="B23" s="105">
-        <f>B$8+(14*A22)</f>
+      <c r="B23" s="60">
+        <f t="shared" si="1"/>
         <v>271</v>
       </c>
-      <c r="C23" s="70">
+      <c r="C23" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D23" s="99"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="70"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="91">
+        <v>-177</v>
+      </c>
+      <c r="D23" s="63">
+        <f>$D$4-B23</f>
+        <v>-85</v>
+      </c>
+      <c r="E23" s="55"/>
+      <c r="F23" s="46"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="52">
         <v>17</v>
       </c>
-      <c r="B24" s="105">
-        <f>B$8+(14*A23)</f>
+      <c r="B24" s="60">
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
-      <c r="C24" s="70">
+      <c r="C24" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="70"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="91">
+        <v>-191</v>
+      </c>
+      <c r="D24" s="63">
+        <f t="shared" si="2"/>
+        <v>-99</v>
+      </c>
+      <c r="E24" s="55"/>
+      <c r="F24" s="46"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="52">
         <v>18</v>
       </c>
-      <c r="B25" s="105">
-        <f>B$8+(14*A24)</f>
+      <c r="B25" s="60">
+        <f t="shared" si="1"/>
         <v>299</v>
       </c>
-      <c r="C25" s="70">
+      <c r="C25" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D25" s="99"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="99"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="70"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="91">
+        <v>-205</v>
+      </c>
+      <c r="D25" s="63">
+        <f t="shared" si="2"/>
+        <v>-113</v>
+      </c>
+      <c r="E25" s="55"/>
+      <c r="F25" s="46"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="52">
         <v>19</v>
       </c>
-      <c r="B26" s="105">
-        <f>B$8+(14*A25)</f>
+      <c r="B26" s="60">
+        <f t="shared" si="1"/>
         <v>313</v>
       </c>
-      <c r="C26" s="70">
+      <c r="C26" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D26" s="99"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="70"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="91">
+        <v>-219</v>
+      </c>
+      <c r="D26" s="63">
+        <f t="shared" si="2"/>
+        <v>-127</v>
+      </c>
+      <c r="E26" s="55"/>
+      <c r="F26" s="46"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="52">
         <v>20</v>
       </c>
-      <c r="B27" s="105">
-        <f>B$8+(14*A26)</f>
+      <c r="B27" s="60">
+        <f t="shared" si="1"/>
         <v>327</v>
       </c>
-      <c r="C27" s="70">
+      <c r="C27" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D27" s="99"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="70"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="91">
+        <v>-233</v>
+      </c>
+      <c r="D27" s="63">
+        <f t="shared" si="2"/>
+        <v>-141</v>
+      </c>
+      <c r="E27" s="55"/>
+      <c r="F27" s="46"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="52">
         <v>21</v>
       </c>
-      <c r="B28" s="105">
-        <f>B$8+(14*A27)</f>
+      <c r="B28" s="60">
+        <f t="shared" si="1"/>
         <v>341</v>
       </c>
-      <c r="C28" s="70">
+      <c r="C28" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D28" s="99"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="70"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="91">
+        <v>-247</v>
+      </c>
+      <c r="D28" s="63">
+        <f t="shared" si="2"/>
+        <v>-155</v>
+      </c>
+      <c r="E28" s="55"/>
+      <c r="F28" s="46"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="52">
         <v>22</v>
       </c>
-      <c r="B29" s="105">
-        <f>B$8+(14*A28)</f>
+      <c r="B29" s="60">
+        <f t="shared" si="1"/>
         <v>355</v>
       </c>
-      <c r="C29" s="70">
+      <c r="C29" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D29" s="99"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="70"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="91">
+        <v>-261</v>
+      </c>
+      <c r="D29" s="63">
+        <f t="shared" si="2"/>
+        <v>-169</v>
+      </c>
+      <c r="E29" s="55"/>
+      <c r="F29" s="46"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="52">
         <v>23</v>
       </c>
-      <c r="B30" s="105">
-        <f>B$8+(14*A29)</f>
+      <c r="B30" s="60">
+        <f t="shared" si="1"/>
         <v>369</v>
       </c>
-      <c r="C30" s="70">
+      <c r="C30" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D30" s="99"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="91">
+        <v>-275</v>
+      </c>
+      <c r="D30" s="63">
+        <f t="shared" si="2"/>
+        <v>-183</v>
+      </c>
+      <c r="E30" s="55"/>
+      <c r="F30" s="46"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="52">
         <v>24</v>
       </c>
-      <c r="B31" s="105">
-        <f>B$8+(14*A30)</f>
+      <c r="B31" s="60">
+        <f t="shared" si="1"/>
         <v>383</v>
       </c>
-      <c r="C31" s="70">
+      <c r="C31" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D31" s="99"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="70"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="91">
+        <v>-289</v>
+      </c>
+      <c r="D31" s="63">
+        <f t="shared" si="2"/>
+        <v>-197</v>
+      </c>
+      <c r="E31" s="55"/>
+      <c r="F31" s="46"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="52">
         <v>25</v>
       </c>
-      <c r="B32" s="105">
-        <f>B$8+(14*A31)</f>
+      <c r="B32" s="60">
+        <f t="shared" si="1"/>
         <v>397</v>
       </c>
-      <c r="C32" s="70">
+      <c r="C32" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D32" s="99"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="70"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="91">
+        <v>-303</v>
+      </c>
+      <c r="D32" s="63">
+        <f t="shared" si="2"/>
+        <v>-211</v>
+      </c>
+      <c r="E32" s="55"/>
+      <c r="F32" s="46"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="52">
         <v>26</v>
       </c>
-      <c r="B33" s="105">
-        <f>B$8+(14*A32)</f>
+      <c r="B33" s="60">
+        <f t="shared" si="1"/>
         <v>411</v>
       </c>
-      <c r="C33" s="70">
+      <c r="C33" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D33" s="99"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="70"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="91">
+        <v>-317</v>
+      </c>
+      <c r="D33" s="63">
+        <f t="shared" si="2"/>
+        <v>-225</v>
+      </c>
+      <c r="E33" s="55"/>
+      <c r="F33" s="46"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="52">
         <v>27</v>
       </c>
-      <c r="B34" s="105">
-        <f>B$8+(14*A33)</f>
+      <c r="B34" s="60">
+        <f t="shared" si="1"/>
         <v>425</v>
       </c>
-      <c r="C34" s="70">
+      <c r="C34" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="70"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="91">
+        <v>-331</v>
+      </c>
+      <c r="D34" s="63">
+        <f t="shared" si="2"/>
+        <v>-239</v>
+      </c>
+      <c r="E34" s="55"/>
+      <c r="F34" s="46"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="52">
         <v>28</v>
       </c>
-      <c r="B35" s="105">
-        <f>B$8+(14*A34)</f>
+      <c r="B35" s="60">
+        <f t="shared" si="1"/>
         <v>439</v>
       </c>
-      <c r="C35" s="70">
+      <c r="C35" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D35" s="99"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="70"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="91">
+        <v>-345</v>
+      </c>
+      <c r="D35" s="63">
+        <f t="shared" si="2"/>
+        <v>-253</v>
+      </c>
+      <c r="E35" s="55"/>
+      <c r="F35" s="46"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="52">
         <v>29</v>
       </c>
-      <c r="B36" s="105">
-        <f>B$8+(14*A35)</f>
+      <c r="B36" s="60">
+        <f t="shared" si="1"/>
         <v>453</v>
       </c>
-      <c r="C36" s="70">
+      <c r="C36" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D36" s="99"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="70"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="91">
+        <v>-359</v>
+      </c>
+      <c r="D36" s="63">
+        <f t="shared" si="2"/>
+        <v>-267</v>
+      </c>
+      <c r="E36" s="55"/>
+      <c r="F36" s="46"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="52">
         <v>30</v>
       </c>
-      <c r="B37" s="105">
-        <f>B$8+(14*A36)</f>
+      <c r="B37" s="60">
+        <f t="shared" si="1"/>
         <v>467</v>
       </c>
-      <c r="C37" s="70">
+      <c r="C37" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D37" s="99"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="70"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="91">
+        <v>-373</v>
+      </c>
+      <c r="D37" s="63">
+        <f t="shared" si="2"/>
+        <v>-281</v>
+      </c>
+      <c r="E37" s="55"/>
+      <c r="F37" s="46"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="52">
         <v>31</v>
       </c>
-      <c r="B38" s="105">
-        <f>B$8+(14*A37)</f>
+      <c r="B38" s="60">
+        <f t="shared" si="1"/>
         <v>481</v>
       </c>
-      <c r="C38" s="70">
+      <c r="C38" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D38" s="99"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="70"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="91">
+        <v>-387</v>
+      </c>
+      <c r="D38" s="63">
+        <f t="shared" si="2"/>
+        <v>-295</v>
+      </c>
+      <c r="E38" s="55"/>
+      <c r="F38" s="46"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="52">
         <v>32</v>
       </c>
-      <c r="B39" s="105">
-        <f>B$8+(14*A38)</f>
+      <c r="B39" s="60">
+        <f t="shared" si="1"/>
         <v>495</v>
       </c>
-      <c r="C39" s="70">
+      <c r="C39" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D39" s="99"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="70"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="91">
+        <v>-401</v>
+      </c>
+      <c r="D39" s="63">
+        <f>$D$4-B39</f>
+        <v>-309</v>
+      </c>
+      <c r="E39" s="55"/>
+      <c r="F39" s="46"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="52">
         <v>33</v>
       </c>
-      <c r="B40" s="105">
-        <f>B$8+(14*A39)</f>
+      <c r="B40" s="60">
+        <f t="shared" si="1"/>
         <v>509</v>
       </c>
-      <c r="C40" s="70">
+      <c r="C40" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D40" s="99"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="70"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="91">
+        <v>-415</v>
+      </c>
+      <c r="D40" s="63">
+        <f t="shared" si="2"/>
+        <v>-323</v>
+      </c>
+      <c r="E40" s="55"/>
+      <c r="F40" s="46"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="52">
         <v>34</v>
       </c>
-      <c r="B41" s="105">
-        <f>B$8+(14*A40)</f>
+      <c r="B41" s="60">
+        <f t="shared" si="1"/>
         <v>523</v>
       </c>
-      <c r="C41" s="70">
+      <c r="C41" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D41" s="99"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="70"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="91">
+        <v>-429</v>
+      </c>
+      <c r="D41" s="63">
+        <f t="shared" si="2"/>
+        <v>-337</v>
+      </c>
+      <c r="E41" s="55"/>
+      <c r="F41" s="46"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="52">
         <v>35</v>
       </c>
-      <c r="B42" s="105">
-        <f>B$8+(14*A41)</f>
+      <c r="B42" s="60">
+        <f t="shared" si="1"/>
         <v>537</v>
       </c>
-      <c r="C42" s="70">
+      <c r="C42" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D42" s="99"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="99"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="70"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="91">
+        <v>-443</v>
+      </c>
+      <c r="D42" s="63">
+        <f t="shared" si="2"/>
+        <v>-351</v>
+      </c>
+      <c r="E42" s="55"/>
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="52">
         <v>36</v>
       </c>
-      <c r="B43" s="105">
-        <f>B$8+(14*A42)</f>
+      <c r="B43" s="60">
+        <f t="shared" si="1"/>
         <v>551</v>
       </c>
-      <c r="C43" s="70">
+      <c r="C43" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D43" s="99"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="99"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="70"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="91">
+        <v>-457</v>
+      </c>
+      <c r="D43" s="63">
+        <f t="shared" si="2"/>
+        <v>-365</v>
+      </c>
+      <c r="E43" s="55"/>
+      <c r="F43" s="46"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="52">
         <v>37</v>
       </c>
-      <c r="B44" s="105">
-        <f>B$8+(14*A43)</f>
+      <c r="B44" s="60">
+        <f t="shared" si="1"/>
         <v>565</v>
       </c>
-      <c r="C44" s="70">
+      <c r="C44" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D44" s="99"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="99"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="70"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="91">
+        <v>-471</v>
+      </c>
+      <c r="D44" s="63">
+        <f t="shared" si="2"/>
+        <v>-379</v>
+      </c>
+      <c r="E44" s="55"/>
+      <c r="F44" s="46"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="52">
         <v>38</v>
       </c>
-      <c r="B45" s="105">
-        <f>B$8+(14*A44)</f>
+      <c r="B45" s="60">
+        <f t="shared" si="1"/>
         <v>579</v>
       </c>
-      <c r="C45" s="70">
+      <c r="C45" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D45" s="99"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="99"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="70"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="91">
+        <v>-485</v>
+      </c>
+      <c r="D45" s="63">
+        <f t="shared" si="2"/>
+        <v>-393</v>
+      </c>
+      <c r="E45" s="55"/>
+      <c r="F45" s="46"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="52">
         <v>39</v>
       </c>
-      <c r="B46" s="105">
-        <f>B$8+(14*A45)</f>
+      <c r="B46" s="60">
+        <f t="shared" si="1"/>
         <v>593</v>
       </c>
-      <c r="C46" s="70">
+      <c r="C46" s="43">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D46" s="99"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="99"/>
-      <c r="H46" s="69"/>
-      <c r="I46" s="70"/>
-    </row>
-    <row r="47" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="92">
+        <v>-499</v>
+      </c>
+      <c r="D46" s="63">
+        <f t="shared" si="2"/>
+        <v>-407</v>
+      </c>
+      <c r="E46" s="55"/>
+      <c r="F46" s="46"/>
+    </row>
+    <row r="47" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="53">
         <v>40</v>
       </c>
-      <c r="B47" s="106">
-        <f>B$8+(14*A46)</f>
+      <c r="B47" s="61">
+        <f t="shared" si="1"/>
         <v>607</v>
       </c>
-      <c r="C47" s="72">
-        <f>(($B$2-1)*14)+$B$8</f>
-        <v>47</v>
-      </c>
-      <c r="D47" s="100"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="100"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="72"/>
+      <c r="C47" s="43">
+        <f t="shared" si="0"/>
+        <v>-513</v>
+      </c>
+      <c r="D47" s="63">
+        <f t="shared" si="2"/>
+        <v>-421</v>
+      </c>
+      <c r="E47" s="56"/>
+      <c r="F47" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="C2:D2"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E2:I5"/>
+    <mergeCell ref="E2:F5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="C2:D2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B8:B47">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>(1+ ((B8-61)/14)) &gt; $B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C47">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>B8&gt;C8</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="1" priority="14">
       <formula>COUNTIF($B$2,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G47 B8:D47">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
-      <formula>$B$8+(($B$2-1)*14)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H47">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
-      <formula>$B$8+(($B$2-1)*14)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I47">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
-      <formula>$B$8+(($B$2-1)*14)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:F47">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
-      <formula>$B$8+(($B$2-1)*14)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:C47">
+  <conditionalFormatting sqref="D8:D47">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>B9&gt;C9</formula>
+      <formula>(1+ ((ABS(D8-$D$4)-61)/14)) &gt; $B$2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
alakdiene unsaturation positions for no ring
</commit_message>
<xml_diff>
--- a/CHC-indentification.xlsx
+++ b/CHC-indentification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CHC-identification_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8542AB3F-C6B3-4F6F-8894-BFD09C81FE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A04396-ABE4-4A0E-9F90-E755C6AF69EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E627A05E-6340-4C51-B36C-84944E4086CC}"/>
   </bookViews>
   <sheets>
     <sheet name="CHC-Identification" sheetId="1" r:id="rId1"/>
@@ -890,7 +890,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
   <si>
     <t>Alkane</t>
   </si>
@@ -973,10 +973,10 @@
     <t>A+ (-b)</t>
   </si>
   <si>
-    <t>A2+ (a)</t>
+    <t>2nd pair</t>
   </si>
   <si>
-    <t>A2+ (b)</t>
+    <t>1st pair</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="69">
+  <borders count="74">
     <border>
       <left/>
       <right/>
@@ -1828,21 +1828,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1889,17 +1874,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -2021,6 +1995,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="mediumDashed">
         <color indexed="64"/>
       </left>
@@ -2030,7 +2050,48 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -2040,7 +2101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2160,9 +2221,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2208,73 +2266,49 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="11" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="4" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2349,7 +2383,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2397,7 +2431,58 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2405,7 +2490,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="88">
     <dxf>
       <fill>
         <patternFill>
@@ -2528,6 +2613,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF6600CC"/>
         </patternFill>
       </fill>
@@ -2886,6 +3027,83 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF6600CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3337,47 +3555,47 @@
         <v>3</v>
       </c>
       <c r="B1" s="24"/>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="88" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="89"/>
+      <c r="P1" s="80"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="85" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="87"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="78"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3396,20 +3614,20 @@
       <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="93"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="84"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -3430,24 +3648,24 @@
         <f>D4-2</f>
         <v>39</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95" t="s">
+      <c r="G4" s="86"/>
+      <c r="H4" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97" t="s">
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="99"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="90"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -3809,20 +4027,20 @@
         <f t="shared" si="8"/>
         <v>165</v>
       </c>
-      <c r="F13" s="91" t="s">
+      <c r="F13" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="92"/>
-      <c r="O13" s="92"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="93"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="83"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="83"/>
+      <c r="P13" s="83"/>
+      <c r="Q13" s="84"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="11">
@@ -3836,24 +4054,24 @@
         <f t="shared" si="9"/>
         <v>179</v>
       </c>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95" t="s">
+      <c r="G14" s="86"/>
+      <c r="H14" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
-      <c r="K14" s="96"/>
-      <c r="L14" s="97" t="s">
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="98"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="98"/>
-      <c r="P14" s="98"/>
-      <c r="Q14" s="99"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="90"/>
     </row>
     <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="C15" s="11">
@@ -4365,40 +4583,40 @@
       </c>
     </row>
     <row r="34" spans="6:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="90" t="s">
+      <c r="F34" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="90"/>
-      <c r="H34" s="90"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="90"/>
-      <c r="O34" s="90"/>
-      <c r="P34" s="90"/>
-      <c r="Q34" s="90"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="81"/>
     </row>
     <row r="35" spans="6:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="90"/>
-      <c r="H35" s="90" t="s">
+      <c r="G35" s="81"/>
+      <c r="H35" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="90"/>
-      <c r="J35" s="90"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90" t="s">
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="90"/>
-      <c r="N35" s="90"/>
-      <c r="O35" s="90"/>
-      <c r="P35" s="90"/>
-      <c r="Q35" s="90"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="81"/>
+      <c r="O35" s="81"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="81"/>
     </row>
     <row r="36" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F36" s="35" t="e" cm="1">
@@ -4620,262 +4838,262 @@
     <mergeCell ref="F13:Q13"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="expression" dxfId="68" priority="108">
+    <cfRule type="expression" dxfId="76" priority="108">
       <formula>COUNTIF($B$1,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C31">
-    <cfRule type="cellIs" dxfId="67" priority="201" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="201" operator="greaterThanOrEqual">
       <formula>$B$3-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D31">
-    <cfRule type="cellIs" dxfId="66" priority="200" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="200" operator="greaterThanOrEqual">
       <formula>$B$4-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E31">
-    <cfRule type="cellIs" dxfId="65" priority="198" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="73" priority="198" operator="greaterThanOrEqual">
       <formula>$B$5-14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16">
-    <cfRule type="expression" dxfId="64" priority="41">
+    <cfRule type="expression" dxfId="72" priority="41">
       <formula>COUNTIF($G$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:G18">
-    <cfRule type="expression" dxfId="63" priority="5">
+    <cfRule type="expression" dxfId="71" priority="5">
       <formula>COUNTIF($G$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:G20">
-    <cfRule type="expression" dxfId="62" priority="4">
+    <cfRule type="expression" dxfId="70" priority="4">
       <formula>COUNTIF($G$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:G22">
-    <cfRule type="expression" dxfId="61" priority="3">
+    <cfRule type="expression" dxfId="69" priority="3">
       <formula>COUNTIF($G$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="60" priority="97">
+    <cfRule type="expression" dxfId="68" priority="97">
       <formula>COUNTIF(F$6:G$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="59" priority="86">
+    <cfRule type="expression" dxfId="67" priority="86">
       <formula>COUNTIF(F8:G8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="58" priority="68">
+    <cfRule type="expression" dxfId="66" priority="68">
       <formula>COUNTIF(F10:G10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="57" priority="67">
+    <cfRule type="expression" dxfId="65" priority="67">
       <formula>COUNTIF(F12:G12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:I16">
-    <cfRule type="expression" dxfId="56" priority="2">
+    <cfRule type="expression" dxfId="64" priority="2">
       <formula>COUNTIF($I$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:I18">
-    <cfRule type="expression" dxfId="55" priority="36">
+    <cfRule type="expression" dxfId="63" priority="36">
       <formula>COUNTIF($I$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:I20">
-    <cfRule type="expression" dxfId="54" priority="35">
+    <cfRule type="expression" dxfId="62" priority="35">
       <formula>COUNTIF($I$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="expression" dxfId="53" priority="34">
+    <cfRule type="expression" dxfId="61" priority="34">
       <formula>COUNTIF($I$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="52" priority="65">
+    <cfRule type="expression" dxfId="60" priority="65">
       <formula>COUNTIF(H$6:I$6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="51" priority="60">
+    <cfRule type="expression" dxfId="59" priority="60">
       <formula>COUNTIF(H8:I8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="50" priority="57">
+    <cfRule type="expression" dxfId="58" priority="57">
       <formula>COUNTIF(H10:I10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="49" priority="56">
+    <cfRule type="expression" dxfId="57" priority="56">
       <formula>COUNTIF(H12:I12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16">
-    <cfRule type="expression" dxfId="48" priority="1">
+    <cfRule type="expression" dxfId="56" priority="1">
       <formula>COUNTIF($K$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18">
-    <cfRule type="expression" dxfId="47" priority="32">
+    <cfRule type="expression" dxfId="55" priority="32">
       <formula>COUNTIF($K$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="expression" dxfId="46" priority="31">
+    <cfRule type="expression" dxfId="54" priority="31">
       <formula>COUNTIF($K$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="expression" dxfId="45" priority="30">
+    <cfRule type="expression" dxfId="53" priority="30">
       <formula>COUNTIF($K$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="44" priority="90">
+    <cfRule type="expression" dxfId="52" priority="90">
       <formula>COUNTIF(J6:K6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="43" priority="52">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>COUNTIF(J8:K8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="42" priority="54">
+    <cfRule type="expression" dxfId="50" priority="54">
       <formula>COUNTIF(J10:K10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="41" priority="53">
+    <cfRule type="expression" dxfId="49" priority="53">
       <formula>COUNTIF(J12:K12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:M16">
-    <cfRule type="expression" dxfId="40" priority="17">
+    <cfRule type="expression" dxfId="48" priority="17">
       <formula>COUNTIF($M$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:M18">
-    <cfRule type="expression" dxfId="39" priority="14">
+    <cfRule type="expression" dxfId="47" priority="14">
       <formula>COUNTIF($M$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:M20">
-    <cfRule type="expression" dxfId="38" priority="13">
+    <cfRule type="expression" dxfId="46" priority="13">
       <formula>COUNTIF($M$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:M22">
-    <cfRule type="expression" dxfId="37" priority="12">
+    <cfRule type="expression" dxfId="45" priority="12">
       <formula>COUNTIF($M$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="36" priority="89">
+    <cfRule type="expression" dxfId="44" priority="89">
       <formula>COUNTIF(L6:M6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="35" priority="50">
+    <cfRule type="expression" dxfId="43" priority="50">
       <formula>COUNTIF(L8:M8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="expression" dxfId="34" priority="49">
+    <cfRule type="expression" dxfId="42" priority="49">
       <formula>COUNTIF(L10:M10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="33" priority="48">
+    <cfRule type="expression" dxfId="41" priority="48">
       <formula>COUNTIF(L12:M12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:O16">
-    <cfRule type="expression" dxfId="32" priority="16">
+    <cfRule type="expression" dxfId="40" priority="16">
       <formula>COUNTIF($O$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:O18">
-    <cfRule type="expression" dxfId="31" priority="11">
+    <cfRule type="expression" dxfId="39" priority="11">
       <formula>COUNTIF($O$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:O20">
-    <cfRule type="expression" dxfId="30" priority="10">
+    <cfRule type="expression" dxfId="38" priority="10">
       <formula>COUNTIF($O$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:O22">
-    <cfRule type="expression" dxfId="29" priority="9">
+    <cfRule type="expression" dxfId="37" priority="9">
       <formula>COUNTIF($O$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="28" priority="88">
+    <cfRule type="expression" dxfId="36" priority="88">
       <formula>COUNTIF(N6:O6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="27" priority="47">
+    <cfRule type="expression" dxfId="35" priority="47">
       <formula>COUNTIF(N8:O8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="26" priority="46">
+    <cfRule type="expression" dxfId="34" priority="46">
       <formula>COUNTIF(N10:O10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="expression" dxfId="25" priority="45">
+    <cfRule type="expression" dxfId="33" priority="45">
       <formula>COUNTIF(N12:O12,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:Q16">
-    <cfRule type="expression" dxfId="24" priority="15">
+    <cfRule type="expression" dxfId="32" priority="15">
       <formula>COUNTIF($Q$15,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="23" priority="8">
+    <cfRule type="expression" dxfId="31" priority="8">
       <formula>COUNTIF($Q$17,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:Q20">
-    <cfRule type="expression" dxfId="22" priority="7">
+    <cfRule type="expression" dxfId="30" priority="7">
       <formula>COUNTIF($Q$19,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:Q22">
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>COUNTIF($Q$21,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="20" priority="87">
+    <cfRule type="expression" dxfId="28" priority="87">
       <formula>COUNTIF(P6:Q6,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="expression" dxfId="19" priority="44">
+    <cfRule type="expression" dxfId="27" priority="44">
       <formula>COUNTIF(P8:Q8,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9">
-    <cfRule type="expression" dxfId="18" priority="43">
+    <cfRule type="expression" dxfId="26" priority="43">
       <formula>COUNTIF(P10:Q10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="expression" dxfId="17" priority="42">
+    <cfRule type="expression" dxfId="25" priority="42">
       <formula>COUNTIF(P12:Q12,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4914,27 +5132,27 @@
       <c r="A1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="101"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4950,1272 +5168,1790 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A751E-AC0F-4038-95D2-ABBAAB30BEF5}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="17.7109375" style="40" customWidth="1"/>
-    <col min="10" max="13" width="1.5703125" style="40" customWidth="1"/>
-    <col min="14" max="15" width="10.5703125" style="40" customWidth="1"/>
-    <col min="16" max="16384" width="10.140625" style="40"/>
+    <col min="1" max="11" width="17.7109375" style="40" customWidth="1"/>
+    <col min="12" max="15" width="1.5703125" style="40" customWidth="1"/>
+    <col min="16" max="17" width="10.5703125" style="40" customWidth="1"/>
+    <col min="18" max="16384" width="10.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="39" customFormat="1" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:17" s="39" customFormat="1" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="102" t="s">
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="102"/>
-    </row>
-    <row r="2" spans="1:15" s="39" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="117" t="s">
+      <c r="Q1" s="93"/>
+    </row>
+    <row r="2" spans="1:17" s="39" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="103" t="s">
+      <c r="B2" s="105"/>
+      <c r="C2" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-    </row>
-    <row r="3" spans="1:15" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="118"/>
-      <c r="B3" s="115"/>
-      <c r="C3" s="41" t="s">
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+    </row>
+    <row r="3" spans="1:17" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="109"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="42">
+      <c r="D3" s="123"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="41">
         <f>B2*14+94</f>
         <v>94</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-    </row>
-    <row r="4" spans="1:15" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118"/>
-      <c r="B4" s="115"/>
-      <c r="C4" s="41" t="s">
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+    </row>
+    <row r="4" spans="1:17" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="109"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="42">
+      <c r="D4" s="123"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="41">
         <f>F3+92</f>
         <v>186</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-    </row>
-    <row r="5" spans="1:15" s="39" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="119"/>
-      <c r="B5" s="116"/>
-      <c r="C5" s="43" t="s">
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+    </row>
+    <row r="5" spans="1:17" s="39" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="110"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
       <c r="J5" s="61"/>
       <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-    </row>
-    <row r="6" spans="1:15" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+    </row>
+    <row r="6" spans="1:17" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="110" t="s">
+      <c r="C6" s="104"/>
+      <c r="D6" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
       <c r="G6" s="111"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="111"/>
-    </row>
-    <row r="7" spans="1:15" s="53" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="107"/>
-      <c r="B7" s="57" t="s">
+      <c r="K6" s="102"/>
+    </row>
+    <row r="7" spans="1:17" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="115"/>
+      <c r="B7" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="125" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="116"/>
+    </row>
+    <row r="8" spans="1:17" s="52" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="98"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F8" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="48" t="s">
+      <c r="G8" s="127" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="J8" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="48" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="50">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="49">
         <v>1</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B9" s="56">
         <v>61</v>
       </c>
-      <c r="C8" s="42">
-        <f>$F$3-B8</f>
+      <c r="C9" s="41">
+        <f>$F$3-B9</f>
         <v>33</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D9" s="49">
         <v>1</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E9" s="65">
         <v>61</v>
       </c>
-      <c r="F8" s="76">
-        <f t="shared" ref="F8:F47" si="0">$F$4-B8-94</f>
+      <c r="F9" s="70">
+        <f>$F$4-B9-94</f>
         <v>31</v>
       </c>
-      <c r="G8" s="77"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="47"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="51">
+      <c r="G9" s="124">
+        <f>$B$2-D9</f>
+        <v>-1</v>
+      </c>
+      <c r="H9" s="70">
+        <f>$F$4-E9-94</f>
+        <v>31</v>
+      </c>
+      <c r="I9" s="56">
+        <v>61</v>
+      </c>
+      <c r="J9" s="55"/>
+      <c r="K9" s="46"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="50">
         <v>2</v>
       </c>
-      <c r="B9" s="59">
-        <f>B$8+(14*A8)</f>
+      <c r="B10" s="57">
+        <f>B$9+(14*A9)</f>
         <v>75</v>
       </c>
-      <c r="C9" s="42">
-        <f t="shared" ref="C9:C47" si="1">$F$3-B9</f>
+      <c r="C10" s="41">
+        <f t="shared" ref="C10:C48" si="0">$F$3-B10</f>
         <v>19</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D10" s="50">
         <v>2</v>
       </c>
-      <c r="E9" s="72">
-        <f>E$8+(14*D8)</f>
+      <c r="E10" s="67">
+        <f>E$9+(14*D9)</f>
         <v>75</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F10" s="70">
+        <f>$F$4-B10-94</f>
+        <v>17</v>
+      </c>
+      <c r="G10" s="124">
+        <f t="shared" ref="G10:G48" si="1">$B$2-D10</f>
+        <v>-2</v>
+      </c>
+      <c r="H10" s="70">
+        <f>$F$4-E10-94</f>
+        <v>17</v>
+      </c>
+      <c r="I10" s="57">
+        <f>I$9+(14*D9)</f>
+        <v>75</v>
+      </c>
+      <c r="J10" s="53"/>
+      <c r="K10" s="44"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="50">
+        <v>3</v>
+      </c>
+      <c r="B11" s="57">
+        <f>B$9+(14*A10)</f>
+        <v>89</v>
+      </c>
+      <c r="C11" s="41">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="G9" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="54"/>
-      <c r="I9" s="45"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="51">
+        <v>5</v>
+      </c>
+      <c r="D11" s="50">
         <v>3</v>
       </c>
-      <c r="B10" s="59">
-        <f t="shared" ref="B10:B47" si="2">B$8+(14*A9)</f>
+      <c r="E11" s="67">
+        <f t="shared" ref="E11:E48" si="2">E$9+(14*D10)</f>
         <v>89</v>
       </c>
-      <c r="C10" s="42">
+      <c r="F11" s="70">
+        <f t="shared" ref="F11:F48" si="3">$F$4-B11-94</f>
+        <v>3</v>
+      </c>
+      <c r="G11" s="124">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="D10" s="51">
+        <v>-3</v>
+      </c>
+      <c r="H11" s="70">
+        <f>$F$4-E11-94</f>
         <v>3</v>
       </c>
-      <c r="E10" s="72">
-        <f t="shared" ref="E10:E47" si="3">E$8+(14*D9)</f>
+      <c r="I11" s="57">
+        <f>I$9+(14*D10)</f>
         <v>89</v>
       </c>
-      <c r="F10" s="76">
+      <c r="J11" s="53"/>
+      <c r="K11" s="44"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="50">
+        <v>4</v>
+      </c>
+      <c r="B12" s="57">
+        <f>B$9+(14*A11)</f>
+        <v>103</v>
+      </c>
+      <c r="C12" s="41">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G10" s="71">
-        <f>B2-(((G8-15-60)/14)+2)</f>
-        <v>3.3571428571428568</v>
-      </c>
-      <c r="H10" s="54"/>
-      <c r="I10" s="45"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="51">
+        <v>-9</v>
+      </c>
+      <c r="D12" s="50">
         <v>4</v>
       </c>
-      <c r="B11" s="59">
+      <c r="E12" s="67">
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
-      <c r="C11" s="42">
+      <c r="F12" s="70">
+        <f t="shared" si="3"/>
+        <v>-11</v>
+      </c>
+      <c r="G12" s="124">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="H12" s="70">
+        <f>$F$4-E12-94</f>
+        <v>-11</v>
+      </c>
+      <c r="I12" s="57">
+        <f>I$9+(14*D11)</f>
+        <v>103</v>
+      </c>
+      <c r="J12" s="53"/>
+      <c r="K12" s="44"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="50">
+        <v>5</v>
+      </c>
+      <c r="B13" s="57">
+        <f>B$9+(14*A12)</f>
+        <v>117</v>
+      </c>
+      <c r="C13" s="41">
+        <f t="shared" si="0"/>
+        <v>-23</v>
+      </c>
+      <c r="D13" s="50">
+        <v>5</v>
+      </c>
+      <c r="E13" s="67">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="F13" s="70">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+      <c r="G13" s="124">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="H13" s="70">
+        <f>$F$4-E13-94</f>
+        <v>-25</v>
+      </c>
+      <c r="I13" s="57">
+        <f>I$9+(14*D12)</f>
+        <v>117</v>
+      </c>
+      <c r="J13" s="53"/>
+      <c r="K13" s="44"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="50">
+        <v>6</v>
+      </c>
+      <c r="B14" s="57">
+        <f>B$9+(14*A13)</f>
+        <v>131</v>
+      </c>
+      <c r="C14" s="41">
+        <f t="shared" si="0"/>
+        <v>-37</v>
+      </c>
+      <c r="D14" s="50">
+        <v>6</v>
+      </c>
+      <c r="E14" s="67">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="F14" s="66">
+        <f t="shared" si="3"/>
+        <v>-39</v>
+      </c>
+      <c r="G14" s="124">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="H14" s="66">
+        <f>$F$4-E14-94</f>
+        <v>-39</v>
+      </c>
+      <c r="I14" s="57">
+        <f>I$9+(14*D13)</f>
+        <v>131</v>
+      </c>
+      <c r="J14" s="53"/>
+      <c r="K14" s="44"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="50">
+        <v>7</v>
+      </c>
+      <c r="B15" s="57">
+        <f>B$9+(14*A14)</f>
+        <v>145</v>
+      </c>
+      <c r="C15" s="41">
+        <f t="shared" si="0"/>
+        <v>-51</v>
+      </c>
+      <c r="D15" s="50">
+        <v>7</v>
+      </c>
+      <c r="E15" s="67">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="F15" s="66">
+        <f t="shared" si="3"/>
+        <v>-53</v>
+      </c>
+      <c r="G15" s="124">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="H15" s="66">
+        <f>$F$4-E15-94</f>
+        <v>-53</v>
+      </c>
+      <c r="I15" s="57">
+        <f>I$9+(14*D14)</f>
+        <v>145</v>
+      </c>
+      <c r="J15" s="53"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="50">
+        <v>8</v>
+      </c>
+      <c r="B16" s="57">
+        <f>B$9+(14*A15)</f>
+        <v>159</v>
+      </c>
+      <c r="C16" s="41">
+        <f t="shared" si="0"/>
+        <v>-65</v>
+      </c>
+      <c r="D16" s="50">
+        <v>8</v>
+      </c>
+      <c r="E16" s="67">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="F16" s="66">
+        <f t="shared" si="3"/>
+        <v>-67</v>
+      </c>
+      <c r="G16" s="124">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="H16" s="66">
+        <f>$F$4-E16-94</f>
+        <v>-67</v>
+      </c>
+      <c r="I16" s="57">
+        <f>I$9+(14*D15)</f>
+        <v>159</v>
+      </c>
+      <c r="J16" s="53"/>
+      <c r="K16" s="44"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="50">
+        <v>9</v>
+      </c>
+      <c r="B17" s="57">
+        <f>B$9+(14*A16)</f>
+        <v>173</v>
+      </c>
+      <c r="C17" s="41">
+        <f t="shared" si="0"/>
+        <v>-79</v>
+      </c>
+      <c r="D17" s="50">
+        <v>9</v>
+      </c>
+      <c r="E17" s="67">
+        <f>E$9+(14*D16)</f>
+        <v>173</v>
+      </c>
+      <c r="F17" s="66">
+        <f>$F$4-B17-94</f>
+        <v>-81</v>
+      </c>
+      <c r="G17" s="124">
         <f t="shared" si="1"/>
         <v>-9</v>
       </c>
-      <c r="D11" s="51">
-        <v>4</v>
-      </c>
-      <c r="E11" s="72">
+      <c r="H17" s="66">
+        <f>$F$4-E17-94</f>
+        <v>-81</v>
+      </c>
+      <c r="I17" s="57">
+        <f>I$9+(14*D16)</f>
+        <v>173</v>
+      </c>
+      <c r="J17" s="53"/>
+      <c r="K17" s="44"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="50">
+        <v>10</v>
+      </c>
+      <c r="B18" s="57">
+        <f>B$9+(14*A17)</f>
+        <v>187</v>
+      </c>
+      <c r="C18" s="41">
+        <f t="shared" si="0"/>
+        <v>-93</v>
+      </c>
+      <c r="D18" s="50">
+        <v>10</v>
+      </c>
+      <c r="E18" s="67">
+        <f t="shared" si="2"/>
+        <v>187</v>
+      </c>
+      <c r="F18" s="66">
         <f t="shared" si="3"/>
-        <v>103</v>
-      </c>
-      <c r="F11" s="76">
+        <v>-95</v>
+      </c>
+      <c r="G18" s="124">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="H18" s="66">
+        <f>$F$4-E18-94</f>
+        <v>-95</v>
+      </c>
+      <c r="I18" s="57">
+        <f>I$9+(14*D17)</f>
+        <v>187</v>
+      </c>
+      <c r="J18" s="53"/>
+      <c r="K18" s="44"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="50">
+        <v>11</v>
+      </c>
+      <c r="B19" s="57">
+        <f>B$9+(14*A18)</f>
+        <v>201</v>
+      </c>
+      <c r="C19" s="41">
         <f t="shared" si="0"/>
+        <v>-107</v>
+      </c>
+      <c r="D19" s="50">
+        <v>11</v>
+      </c>
+      <c r="E19" s="67">
+        <f t="shared" si="2"/>
+        <v>201</v>
+      </c>
+      <c r="F19" s="66">
+        <f t="shared" si="3"/>
+        <v>-109</v>
+      </c>
+      <c r="G19" s="124">
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
-      <c r="G11" s="78" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="45"/>
-    </row>
-    <row r="12" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51">
-        <v>5</v>
-      </c>
-      <c r="B12" s="59">
+      <c r="H19" s="66">
+        <f>$F$4-E19-94</f>
+        <v>-109</v>
+      </c>
+      <c r="I19" s="57">
+        <f>I$9+(14*D18)</f>
+        <v>201</v>
+      </c>
+      <c r="J19" s="53"/>
+      <c r="K19" s="44"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="50">
+        <v>12</v>
+      </c>
+      <c r="B20" s="57">
+        <f>B$9+(14*A19)</f>
+        <v>215</v>
+      </c>
+      <c r="C20" s="41">
+        <f t="shared" si="0"/>
+        <v>-121</v>
+      </c>
+      <c r="D20" s="50">
+        <v>12</v>
+      </c>
+      <c r="E20" s="67">
         <f t="shared" si="2"/>
-        <v>117</v>
-      </c>
-      <c r="C12" s="42">
+        <v>215</v>
+      </c>
+      <c r="F20" s="66">
+        <f t="shared" si="3"/>
+        <v>-123</v>
+      </c>
+      <c r="G20" s="124">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="H20" s="66">
+        <f>$F$4-E20-94</f>
+        <v>-123</v>
+      </c>
+      <c r="I20" s="57">
+        <f>I$9+(14*D19)</f>
+        <v>215</v>
+      </c>
+      <c r="J20" s="53"/>
+      <c r="K20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="50">
+        <v>13</v>
+      </c>
+      <c r="B21" s="57">
+        <f>B$9+(14*A20)</f>
+        <v>229</v>
+      </c>
+      <c r="C21" s="41">
+        <f t="shared" si="0"/>
+        <v>-135</v>
+      </c>
+      <c r="D21" s="50">
+        <v>13</v>
+      </c>
+      <c r="E21" s="67">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
+      <c r="F21" s="66">
+        <f t="shared" si="3"/>
+        <v>-137</v>
+      </c>
+      <c r="G21" s="124">
+        <f t="shared" si="1"/>
+        <v>-13</v>
+      </c>
+      <c r="H21" s="66">
+        <f>$F$4-E21-94</f>
+        <v>-137</v>
+      </c>
+      <c r="I21" s="57">
+        <f>I$9+(14*D20)</f>
+        <v>229</v>
+      </c>
+      <c r="J21" s="53"/>
+      <c r="K21" s="44"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="50">
+        <v>14</v>
+      </c>
+      <c r="B22" s="57">
+        <f>B$9+(14*A21)</f>
+        <v>243</v>
+      </c>
+      <c r="C22" s="41">
+        <f t="shared" si="0"/>
+        <v>-149</v>
+      </c>
+      <c r="D22" s="50">
+        <v>14</v>
+      </c>
+      <c r="E22" s="67">
+        <f t="shared" si="2"/>
+        <v>243</v>
+      </c>
+      <c r="F22" s="66">
+        <f t="shared" si="3"/>
+        <v>-151</v>
+      </c>
+      <c r="G22" s="124">
+        <f t="shared" si="1"/>
+        <v>-14</v>
+      </c>
+      <c r="H22" s="66">
+        <f>$F$4-E22-94</f>
+        <v>-151</v>
+      </c>
+      <c r="I22" s="57">
+        <f>I$9+(14*D21)</f>
+        <v>243</v>
+      </c>
+      <c r="J22" s="53"/>
+      <c r="K22" s="44"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="50">
+        <v>15</v>
+      </c>
+      <c r="B23" s="57">
+        <f>B$9+(14*A22)</f>
+        <v>257</v>
+      </c>
+      <c r="C23" s="41">
+        <f t="shared" si="0"/>
+        <v>-163</v>
+      </c>
+      <c r="D23" s="50">
+        <v>15</v>
+      </c>
+      <c r="E23" s="67">
+        <f t="shared" si="2"/>
+        <v>257</v>
+      </c>
+      <c r="F23" s="66">
+        <f t="shared" si="3"/>
+        <v>-165</v>
+      </c>
+      <c r="G23" s="124">
+        <f t="shared" si="1"/>
+        <v>-15</v>
+      </c>
+      <c r="H23" s="66">
+        <f>$F$4-E23-94</f>
+        <v>-165</v>
+      </c>
+      <c r="I23" s="57">
+        <f>I$9+(14*D22)</f>
+        <v>257</v>
+      </c>
+      <c r="J23" s="53"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="50">
+        <v>16</v>
+      </c>
+      <c r="B24" s="57">
+        <f>B$9+(14*A23)</f>
+        <v>271</v>
+      </c>
+      <c r="C24" s="41">
+        <f t="shared" si="0"/>
+        <v>-177</v>
+      </c>
+      <c r="D24" s="50">
+        <v>16</v>
+      </c>
+      <c r="E24" s="67">
+        <f t="shared" si="2"/>
+        <v>271</v>
+      </c>
+      <c r="F24" s="66">
+        <f t="shared" si="3"/>
+        <v>-179</v>
+      </c>
+      <c r="G24" s="124">
+        <f t="shared" si="1"/>
+        <v>-16</v>
+      </c>
+      <c r="H24" s="66">
+        <f>$F$4-E24-94</f>
+        <v>-179</v>
+      </c>
+      <c r="I24" s="57">
+        <f>I$9+(14*D23)</f>
+        <v>271</v>
+      </c>
+      <c r="J24" s="53"/>
+      <c r="K24" s="44"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="50">
+        <v>17</v>
+      </c>
+      <c r="B25" s="57">
+        <f>B$9+(14*A24)</f>
+        <v>285</v>
+      </c>
+      <c r="C25" s="41">
+        <f t="shared" si="0"/>
+        <v>-191</v>
+      </c>
+      <c r="D25" s="50">
+        <v>17</v>
+      </c>
+      <c r="E25" s="67">
+        <f t="shared" si="2"/>
+        <v>285</v>
+      </c>
+      <c r="F25" s="66">
+        <f t="shared" si="3"/>
+        <v>-193</v>
+      </c>
+      <c r="G25" s="124">
+        <f t="shared" si="1"/>
+        <v>-17</v>
+      </c>
+      <c r="H25" s="66">
+        <f>$F$4-E25-94</f>
+        <v>-193</v>
+      </c>
+      <c r="I25" s="57">
+        <f>I$9+(14*D24)</f>
+        <v>285</v>
+      </c>
+      <c r="J25" s="53"/>
+      <c r="K25" s="44"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="50">
+        <v>18</v>
+      </c>
+      <c r="B26" s="57">
+        <f>B$9+(14*A25)</f>
+        <v>299</v>
+      </c>
+      <c r="C26" s="41">
+        <f t="shared" si="0"/>
+        <v>-205</v>
+      </c>
+      <c r="D26" s="50">
+        <v>18</v>
+      </c>
+      <c r="E26" s="67">
+        <f t="shared" si="2"/>
+        <v>299</v>
+      </c>
+      <c r="F26" s="66">
+        <f t="shared" si="3"/>
+        <v>-207</v>
+      </c>
+      <c r="G26" s="124">
+        <f t="shared" si="1"/>
+        <v>-18</v>
+      </c>
+      <c r="H26" s="66">
+        <f>$F$4-E26-94</f>
+        <v>-207</v>
+      </c>
+      <c r="I26" s="57">
+        <f>I$9+(14*D25)</f>
+        <v>299</v>
+      </c>
+      <c r="J26" s="53"/>
+      <c r="K26" s="44"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="50">
+        <v>19</v>
+      </c>
+      <c r="B27" s="57">
+        <f>B$9+(14*A26)</f>
+        <v>313</v>
+      </c>
+      <c r="C27" s="41">
+        <f t="shared" si="0"/>
+        <v>-219</v>
+      </c>
+      <c r="D27" s="50">
+        <v>19</v>
+      </c>
+      <c r="E27" s="67">
+        <f t="shared" si="2"/>
+        <v>313</v>
+      </c>
+      <c r="F27" s="66">
+        <f t="shared" si="3"/>
+        <v>-221</v>
+      </c>
+      <c r="G27" s="124">
+        <f t="shared" si="1"/>
+        <v>-19</v>
+      </c>
+      <c r="H27" s="66">
+        <f>$F$4-E27-94</f>
+        <v>-221</v>
+      </c>
+      <c r="I27" s="57">
+        <f>I$9+(14*D26)</f>
+        <v>313</v>
+      </c>
+      <c r="J27" s="53"/>
+      <c r="K27" s="44"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="50">
+        <v>20</v>
+      </c>
+      <c r="B28" s="57">
+        <f>B$9+(14*A27)</f>
+        <v>327</v>
+      </c>
+      <c r="C28" s="41">
+        <f t="shared" si="0"/>
+        <v>-233</v>
+      </c>
+      <c r="D28" s="50">
+        <v>20</v>
+      </c>
+      <c r="E28" s="67">
+        <f t="shared" si="2"/>
+        <v>327</v>
+      </c>
+      <c r="F28" s="66">
+        <f t="shared" si="3"/>
+        <v>-235</v>
+      </c>
+      <c r="G28" s="124">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="H28" s="66">
+        <f>$F$4-E28-94</f>
+        <v>-235</v>
+      </c>
+      <c r="I28" s="57">
+        <f>I$9+(14*D27)</f>
+        <v>327</v>
+      </c>
+      <c r="J28" s="53"/>
+      <c r="K28" s="44"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="50">
+        <v>21</v>
+      </c>
+      <c r="B29" s="57">
+        <f>B$9+(14*A28)</f>
+        <v>341</v>
+      </c>
+      <c r="C29" s="41">
+        <f t="shared" si="0"/>
+        <v>-247</v>
+      </c>
+      <c r="D29" s="50">
+        <v>21</v>
+      </c>
+      <c r="E29" s="67">
+        <f t="shared" si="2"/>
+        <v>341</v>
+      </c>
+      <c r="F29" s="66">
+        <f t="shared" si="3"/>
+        <v>-249</v>
+      </c>
+      <c r="G29" s="124">
+        <f t="shared" si="1"/>
+        <v>-21</v>
+      </c>
+      <c r="H29" s="66">
+        <f>$F$4-E29-94</f>
+        <v>-249</v>
+      </c>
+      <c r="I29" s="57">
+        <f>I$9+(14*D28)</f>
+        <v>341</v>
+      </c>
+      <c r="J29" s="53"/>
+      <c r="K29" s="44"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="50">
+        <v>22</v>
+      </c>
+      <c r="B30" s="57">
+        <f>B$9+(14*A29)</f>
+        <v>355</v>
+      </c>
+      <c r="C30" s="41">
+        <f t="shared" si="0"/>
+        <v>-261</v>
+      </c>
+      <c r="D30" s="50">
+        <v>22</v>
+      </c>
+      <c r="E30" s="67">
+        <f t="shared" si="2"/>
+        <v>355</v>
+      </c>
+      <c r="F30" s="66">
+        <f t="shared" si="3"/>
+        <v>-263</v>
+      </c>
+      <c r="G30" s="124">
+        <f t="shared" si="1"/>
+        <v>-22</v>
+      </c>
+      <c r="H30" s="66">
+        <f>$F$4-E30-94</f>
+        <v>-263</v>
+      </c>
+      <c r="I30" s="57">
+        <f>I$9+(14*D29)</f>
+        <v>355</v>
+      </c>
+      <c r="J30" s="53"/>
+      <c r="K30" s="44"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="50">
+        <v>23</v>
+      </c>
+      <c r="B31" s="57">
+        <f>B$9+(14*A30)</f>
+        <v>369</v>
+      </c>
+      <c r="C31" s="41">
+        <f t="shared" si="0"/>
+        <v>-275</v>
+      </c>
+      <c r="D31" s="50">
+        <v>23</v>
+      </c>
+      <c r="E31" s="67">
+        <f t="shared" si="2"/>
+        <v>369</v>
+      </c>
+      <c r="F31" s="66">
+        <f t="shared" si="3"/>
+        <v>-277</v>
+      </c>
+      <c r="G31" s="124">
         <f t="shared" si="1"/>
         <v>-23</v>
       </c>
-      <c r="D12" s="51">
-        <v>5</v>
-      </c>
-      <c r="E12" s="72">
+      <c r="H31" s="66">
+        <f>$F$4-E31-94</f>
+        <v>-277</v>
+      </c>
+      <c r="I31" s="57">
+        <f>I$9+(14*D30)</f>
+        <v>369</v>
+      </c>
+      <c r="J31" s="53"/>
+      <c r="K31" s="44"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="50">
+        <v>24</v>
+      </c>
+      <c r="B32" s="57">
+        <f>B$9+(14*A31)</f>
+        <v>383</v>
+      </c>
+      <c r="C32" s="41">
+        <f t="shared" si="0"/>
+        <v>-289</v>
+      </c>
+      <c r="D32" s="50">
+        <v>24</v>
+      </c>
+      <c r="E32" s="67">
+        <f t="shared" si="2"/>
+        <v>383</v>
+      </c>
+      <c r="F32" s="66">
         <f t="shared" si="3"/>
-        <v>117</v>
-      </c>
-      <c r="F12" s="76">
+        <v>-291</v>
+      </c>
+      <c r="G32" s="124">
+        <f t="shared" si="1"/>
+        <v>-24</v>
+      </c>
+      <c r="H32" s="66">
+        <f>$F$4-E32-94</f>
+        <v>-291</v>
+      </c>
+      <c r="I32" s="57">
+        <f>I$9+(14*D31)</f>
+        <v>383</v>
+      </c>
+      <c r="J32" s="53"/>
+      <c r="K32" s="44"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="50">
+        <v>25</v>
+      </c>
+      <c r="B33" s="57">
+        <f>B$9+(14*A32)</f>
+        <v>397</v>
+      </c>
+      <c r="C33" s="41">
         <f t="shared" si="0"/>
+        <v>-303</v>
+      </c>
+      <c r="D33" s="50">
+        <v>25</v>
+      </c>
+      <c r="E33" s="67">
+        <f t="shared" si="2"/>
+        <v>397</v>
+      </c>
+      <c r="F33" s="66">
+        <f t="shared" si="3"/>
+        <v>-305</v>
+      </c>
+      <c r="G33" s="124">
+        <f t="shared" si="1"/>
         <v>-25</v>
       </c>
-      <c r="G12" s="79">
-        <f>F4-G8-94</f>
-        <v>92</v>
-      </c>
-      <c r="H12" s="54"/>
-      <c r="I12" s="45"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="51">
-        <v>6</v>
-      </c>
-      <c r="B13" s="59">
+      <c r="H33" s="66">
+        <f>$F$4-E33-94</f>
+        <v>-305</v>
+      </c>
+      <c r="I33" s="57">
+        <f>I$9+(14*D32)</f>
+        <v>397</v>
+      </c>
+      <c r="J33" s="53"/>
+      <c r="K33" s="44"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="50">
+        <v>26</v>
+      </c>
+      <c r="B34" s="57">
+        <f>B$9+(14*A33)</f>
+        <v>411</v>
+      </c>
+      <c r="C34" s="41">
+        <f t="shared" si="0"/>
+        <v>-317</v>
+      </c>
+      <c r="D34" s="50">
+        <v>26</v>
+      </c>
+      <c r="E34" s="67">
         <f t="shared" si="2"/>
-        <v>131</v>
-      </c>
-      <c r="C13" s="42">
+        <v>411</v>
+      </c>
+      <c r="F34" s="66">
+        <f t="shared" si="3"/>
+        <v>-319</v>
+      </c>
+      <c r="G34" s="124">
+        <f t="shared" si="1"/>
+        <v>-26</v>
+      </c>
+      <c r="H34" s="66">
+        <f>$F$4-E34-94</f>
+        <v>-319</v>
+      </c>
+      <c r="I34" s="57">
+        <f>I$9+(14*D33)</f>
+        <v>411</v>
+      </c>
+      <c r="J34" s="53"/>
+      <c r="K34" s="44"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="50">
+        <v>27</v>
+      </c>
+      <c r="B35" s="57">
+        <f>B$9+(14*A34)</f>
+        <v>425</v>
+      </c>
+      <c r="C35" s="41">
+        <f t="shared" si="0"/>
+        <v>-331</v>
+      </c>
+      <c r="D35" s="50">
+        <v>27</v>
+      </c>
+      <c r="E35" s="67">
+        <f t="shared" si="2"/>
+        <v>425</v>
+      </c>
+      <c r="F35" s="66">
+        <f t="shared" si="3"/>
+        <v>-333</v>
+      </c>
+      <c r="G35" s="124">
+        <f t="shared" si="1"/>
+        <v>-27</v>
+      </c>
+      <c r="H35" s="66">
+        <f>$F$4-E35-94</f>
+        <v>-333</v>
+      </c>
+      <c r="I35" s="57">
+        <f>I$9+(14*D34)</f>
+        <v>425</v>
+      </c>
+      <c r="J35" s="53"/>
+      <c r="K35" s="44"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="50">
+        <v>28</v>
+      </c>
+      <c r="B36" s="57">
+        <f>B$9+(14*A35)</f>
+        <v>439</v>
+      </c>
+      <c r="C36" s="41">
+        <f t="shared" si="0"/>
+        <v>-345</v>
+      </c>
+      <c r="D36" s="50">
+        <v>28</v>
+      </c>
+      <c r="E36" s="67">
+        <f t="shared" si="2"/>
+        <v>439</v>
+      </c>
+      <c r="F36" s="66">
+        <f t="shared" si="3"/>
+        <v>-347</v>
+      </c>
+      <c r="G36" s="124">
+        <f t="shared" si="1"/>
+        <v>-28</v>
+      </c>
+      <c r="H36" s="66">
+        <f>$F$4-E36-94</f>
+        <v>-347</v>
+      </c>
+      <c r="I36" s="57">
+        <f>I$9+(14*D35)</f>
+        <v>439</v>
+      </c>
+      <c r="J36" s="53"/>
+      <c r="K36" s="44"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="50">
+        <v>29</v>
+      </c>
+      <c r="B37" s="57">
+        <f>B$9+(14*A36)</f>
+        <v>453</v>
+      </c>
+      <c r="C37" s="41">
+        <f t="shared" si="0"/>
+        <v>-359</v>
+      </c>
+      <c r="D37" s="50">
+        <v>29</v>
+      </c>
+      <c r="E37" s="67">
+        <f t="shared" si="2"/>
+        <v>453</v>
+      </c>
+      <c r="F37" s="66">
+        <f t="shared" si="3"/>
+        <v>-361</v>
+      </c>
+      <c r="G37" s="124">
+        <f t="shared" si="1"/>
+        <v>-29</v>
+      </c>
+      <c r="H37" s="66">
+        <f>$F$4-E37-94</f>
+        <v>-361</v>
+      </c>
+      <c r="I37" s="57">
+        <f>I$9+(14*D36)</f>
+        <v>453</v>
+      </c>
+      <c r="J37" s="53"/>
+      <c r="K37" s="44"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="50">
+        <v>30</v>
+      </c>
+      <c r="B38" s="57">
+        <f>B$9+(14*A37)</f>
+        <v>467</v>
+      </c>
+      <c r="C38" s="41">
+        <f t="shared" si="0"/>
+        <v>-373</v>
+      </c>
+      <c r="D38" s="50">
+        <v>30</v>
+      </c>
+      <c r="E38" s="67">
+        <f t="shared" si="2"/>
+        <v>467</v>
+      </c>
+      <c r="F38" s="66">
+        <f t="shared" si="3"/>
+        <v>-375</v>
+      </c>
+      <c r="G38" s="124">
+        <f t="shared" si="1"/>
+        <v>-30</v>
+      </c>
+      <c r="H38" s="66">
+        <f>$F$4-E38-94</f>
+        <v>-375</v>
+      </c>
+      <c r="I38" s="57">
+        <f>I$9+(14*D37)</f>
+        <v>467</v>
+      </c>
+      <c r="J38" s="53"/>
+      <c r="K38" s="44"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="50">
+        <v>31</v>
+      </c>
+      <c r="B39" s="57">
+        <f>B$9+(14*A38)</f>
+        <v>481</v>
+      </c>
+      <c r="C39" s="41">
+        <f t="shared" si="0"/>
+        <v>-387</v>
+      </c>
+      <c r="D39" s="50">
+        <v>31</v>
+      </c>
+      <c r="E39" s="67">
+        <f t="shared" si="2"/>
+        <v>481</v>
+      </c>
+      <c r="F39" s="66">
+        <f t="shared" si="3"/>
+        <v>-389</v>
+      </c>
+      <c r="G39" s="124">
+        <f t="shared" si="1"/>
+        <v>-31</v>
+      </c>
+      <c r="H39" s="66">
+        <f>$F$4-E39-94</f>
+        <v>-389</v>
+      </c>
+      <c r="I39" s="57">
+        <f>I$9+(14*D38)</f>
+        <v>481</v>
+      </c>
+      <c r="J39" s="53"/>
+      <c r="K39" s="44"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="50">
+        <v>32</v>
+      </c>
+      <c r="B40" s="57">
+        <f>B$9+(14*A39)</f>
+        <v>495</v>
+      </c>
+      <c r="C40" s="41">
+        <f t="shared" si="0"/>
+        <v>-401</v>
+      </c>
+      <c r="D40" s="50">
+        <v>32</v>
+      </c>
+      <c r="E40" s="67">
+        <f t="shared" si="2"/>
+        <v>495</v>
+      </c>
+      <c r="F40" s="66">
+        <f t="shared" si="3"/>
+        <v>-403</v>
+      </c>
+      <c r="G40" s="124">
+        <f t="shared" si="1"/>
+        <v>-32</v>
+      </c>
+      <c r="H40" s="66">
+        <f>$F$4-E40-94</f>
+        <v>-403</v>
+      </c>
+      <c r="I40" s="57">
+        <f>I$9+(14*D39)</f>
+        <v>495</v>
+      </c>
+      <c r="J40" s="53"/>
+      <c r="K40" s="44"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="50">
+        <v>33</v>
+      </c>
+      <c r="B41" s="57">
+        <f>B$9+(14*A40)</f>
+        <v>509</v>
+      </c>
+      <c r="C41" s="41">
+        <f t="shared" si="0"/>
+        <v>-415</v>
+      </c>
+      <c r="D41" s="50">
+        <v>33</v>
+      </c>
+      <c r="E41" s="67">
+        <f t="shared" si="2"/>
+        <v>509</v>
+      </c>
+      <c r="F41" s="66">
+        <f t="shared" si="3"/>
+        <v>-417</v>
+      </c>
+      <c r="G41" s="124">
+        <f t="shared" si="1"/>
+        <v>-33</v>
+      </c>
+      <c r="H41" s="66">
+        <f>$F$4-E41-94</f>
+        <v>-417</v>
+      </c>
+      <c r="I41" s="57">
+        <f>I$9+(14*D40)</f>
+        <v>509</v>
+      </c>
+      <c r="J41" s="53"/>
+      <c r="K41" s="44"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="50">
+        <v>34</v>
+      </c>
+      <c r="B42" s="57">
+        <f>B$9+(14*A41)</f>
+        <v>523</v>
+      </c>
+      <c r="C42" s="41">
+        <f t="shared" si="0"/>
+        <v>-429</v>
+      </c>
+      <c r="D42" s="50">
+        <v>34</v>
+      </c>
+      <c r="E42" s="67">
+        <f t="shared" si="2"/>
+        <v>523</v>
+      </c>
+      <c r="F42" s="66">
+        <f t="shared" si="3"/>
+        <v>-431</v>
+      </c>
+      <c r="G42" s="124">
+        <f t="shared" si="1"/>
+        <v>-34</v>
+      </c>
+      <c r="H42" s="66">
+        <f>$F$4-E42-94</f>
+        <v>-431</v>
+      </c>
+      <c r="I42" s="57">
+        <f>I$9+(14*D41)</f>
+        <v>523</v>
+      </c>
+      <c r="J42" s="53"/>
+      <c r="K42" s="44"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="50">
+        <v>35</v>
+      </c>
+      <c r="B43" s="57">
+        <f>B$9+(14*A42)</f>
+        <v>537</v>
+      </c>
+      <c r="C43" s="41">
+        <f t="shared" si="0"/>
+        <v>-443</v>
+      </c>
+      <c r="D43" s="50">
+        <v>35</v>
+      </c>
+      <c r="E43" s="67">
+        <f t="shared" si="2"/>
+        <v>537</v>
+      </c>
+      <c r="F43" s="66">
+        <f t="shared" si="3"/>
+        <v>-445</v>
+      </c>
+      <c r="G43" s="124">
+        <f t="shared" si="1"/>
+        <v>-35</v>
+      </c>
+      <c r="H43" s="66">
+        <f>$F$4-E43-94</f>
+        <v>-445</v>
+      </c>
+      <c r="I43" s="57">
+        <f>I$9+(14*D42)</f>
+        <v>537</v>
+      </c>
+      <c r="J43" s="53"/>
+      <c r="K43" s="44"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="50">
+        <v>36</v>
+      </c>
+      <c r="B44" s="57">
+        <f>B$9+(14*A43)</f>
+        <v>551</v>
+      </c>
+      <c r="C44" s="41">
+        <f t="shared" si="0"/>
+        <v>-457</v>
+      </c>
+      <c r="D44" s="50">
+        <v>36</v>
+      </c>
+      <c r="E44" s="67">
+        <f t="shared" si="2"/>
+        <v>551</v>
+      </c>
+      <c r="F44" s="66">
+        <f t="shared" si="3"/>
+        <v>-459</v>
+      </c>
+      <c r="G44" s="124">
+        <f t="shared" si="1"/>
+        <v>-36</v>
+      </c>
+      <c r="H44" s="66">
+        <f>$F$4-E44-94</f>
+        <v>-459</v>
+      </c>
+      <c r="I44" s="57">
+        <f>I$9+(14*D43)</f>
+        <v>551</v>
+      </c>
+      <c r="J44" s="53"/>
+      <c r="K44" s="44"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="50">
+        <v>37</v>
+      </c>
+      <c r="B45" s="57">
+        <f>B$9+(14*A44)</f>
+        <v>565</v>
+      </c>
+      <c r="C45" s="41">
+        <f t="shared" si="0"/>
+        <v>-471</v>
+      </c>
+      <c r="D45" s="50">
+        <v>37</v>
+      </c>
+      <c r="E45" s="67">
+        <f t="shared" si="2"/>
+        <v>565</v>
+      </c>
+      <c r="F45" s="66">
+        <f t="shared" si="3"/>
+        <v>-473</v>
+      </c>
+      <c r="G45" s="124">
         <f t="shared" si="1"/>
         <v>-37</v>
       </c>
-      <c r="D13" s="51">
-        <v>6</v>
-      </c>
-      <c r="E13" s="72">
-        <f t="shared" si="3"/>
-        <v>131</v>
-      </c>
-      <c r="F13" s="71">
+      <c r="H45" s="66">
+        <f>$F$4-E45-94</f>
+        <v>-473</v>
+      </c>
+      <c r="I45" s="57">
+        <f>I$9+(14*D44)</f>
+        <v>565</v>
+      </c>
+      <c r="J45" s="53"/>
+      <c r="K45" s="44"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="50">
+        <v>38</v>
+      </c>
+      <c r="B46" s="57">
+        <f>B$9+(14*A45)</f>
+        <v>579</v>
+      </c>
+      <c r="C46" s="41">
         <f t="shared" si="0"/>
-        <v>-39</v>
-      </c>
-      <c r="H13" s="54"/>
-      <c r="I13" s="45"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="51">
-        <v>7</v>
-      </c>
-      <c r="B14" s="59">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="C14" s="42">
-        <f t="shared" si="1"/>
-        <v>-51</v>
-      </c>
-      <c r="D14" s="51">
-        <v>7</v>
-      </c>
-      <c r="E14" s="72">
-        <f t="shared" si="3"/>
-        <v>145</v>
-      </c>
-      <c r="F14" s="71">
-        <f t="shared" si="0"/>
-        <v>-53</v>
-      </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="45"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="51">
-        <v>8</v>
-      </c>
-      <c r="B15" s="59">
-        <f t="shared" si="2"/>
-        <v>159</v>
-      </c>
-      <c r="C15" s="42">
-        <f t="shared" si="1"/>
-        <v>-65</v>
-      </c>
-      <c r="D15" s="51">
-        <v>8</v>
-      </c>
-      <c r="E15" s="72">
-        <f t="shared" si="3"/>
-        <v>159</v>
-      </c>
-      <c r="F15" s="71">
-        <f t="shared" si="0"/>
-        <v>-67</v>
-      </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="45"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="51">
-        <v>9</v>
-      </c>
-      <c r="B16" s="59">
-        <f>B$8+(14*A15)</f>
-        <v>173</v>
-      </c>
-      <c r="C16" s="42">
-        <f t="shared" si="1"/>
-        <v>-79</v>
-      </c>
-      <c r="D16" s="51">
-        <v>9</v>
-      </c>
-      <c r="E16" s="72">
-        <f>E$8+(14*D15)</f>
-        <v>173</v>
-      </c>
-      <c r="F16" s="71">
-        <f t="shared" si="0"/>
-        <v>-81</v>
-      </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="45"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="51">
-        <v>10</v>
-      </c>
-      <c r="B17" s="59">
-        <f t="shared" si="2"/>
-        <v>187</v>
-      </c>
-      <c r="C17" s="42">
-        <f t="shared" si="1"/>
-        <v>-93</v>
-      </c>
-      <c r="D17" s="51">
-        <v>10</v>
-      </c>
-      <c r="E17" s="72">
-        <f t="shared" si="3"/>
-        <v>187</v>
-      </c>
-      <c r="F17" s="71">
-        <f t="shared" si="0"/>
-        <v>-95</v>
-      </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="45"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="51">
-        <v>11</v>
-      </c>
-      <c r="B18" s="59">
-        <f t="shared" si="2"/>
-        <v>201</v>
-      </c>
-      <c r="C18" s="42">
-        <f t="shared" si="1"/>
-        <v>-107</v>
-      </c>
-      <c r="D18" s="51">
-        <v>11</v>
-      </c>
-      <c r="E18" s="72">
-        <f t="shared" si="3"/>
-        <v>201</v>
-      </c>
-      <c r="F18" s="71">
-        <f t="shared" si="0"/>
-        <v>-109</v>
-      </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="45"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="51">
-        <v>12</v>
-      </c>
-      <c r="B19" s="59">
-        <f t="shared" si="2"/>
-        <v>215</v>
-      </c>
-      <c r="C19" s="42">
-        <f t="shared" si="1"/>
-        <v>-121</v>
-      </c>
-      <c r="D19" s="51">
-        <v>12</v>
-      </c>
-      <c r="E19" s="72">
-        <f t="shared" si="3"/>
-        <v>215</v>
-      </c>
-      <c r="F19" s="71">
-        <f t="shared" si="0"/>
-        <v>-123</v>
-      </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="45"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="51">
-        <v>13</v>
-      </c>
-      <c r="B20" s="59">
-        <f t="shared" si="2"/>
-        <v>229</v>
-      </c>
-      <c r="C20" s="42">
-        <f t="shared" si="1"/>
-        <v>-135</v>
-      </c>
-      <c r="D20" s="51">
-        <v>13</v>
-      </c>
-      <c r="E20" s="72">
-        <f t="shared" si="3"/>
-        <v>229</v>
-      </c>
-      <c r="F20" s="71">
-        <f t="shared" si="0"/>
-        <v>-137</v>
-      </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="45"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
-        <v>14</v>
-      </c>
-      <c r="B21" s="59">
-        <f t="shared" si="2"/>
-        <v>243</v>
-      </c>
-      <c r="C21" s="42">
-        <f t="shared" si="1"/>
-        <v>-149</v>
-      </c>
-      <c r="D21" s="51">
-        <v>14</v>
-      </c>
-      <c r="E21" s="72">
-        <f t="shared" si="3"/>
-        <v>243</v>
-      </c>
-      <c r="F21" s="71">
-        <f t="shared" si="0"/>
-        <v>-151</v>
-      </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="45"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="51">
-        <v>15</v>
-      </c>
-      <c r="B22" s="59">
-        <f t="shared" si="2"/>
-        <v>257</v>
-      </c>
-      <c r="C22" s="42">
-        <f t="shared" si="1"/>
-        <v>-163</v>
-      </c>
-      <c r="D22" s="51">
-        <v>15</v>
-      </c>
-      <c r="E22" s="72">
-        <f t="shared" si="3"/>
-        <v>257</v>
-      </c>
-      <c r="F22" s="71">
-        <f t="shared" si="0"/>
-        <v>-165</v>
-      </c>
-      <c r="H22" s="54"/>
-      <c r="I22" s="45"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="51">
-        <v>16</v>
-      </c>
-      <c r="B23" s="59">
-        <f t="shared" si="2"/>
-        <v>271</v>
-      </c>
-      <c r="C23" s="42">
-        <f t="shared" si="1"/>
-        <v>-177</v>
-      </c>
-      <c r="D23" s="51">
-        <v>16</v>
-      </c>
-      <c r="E23" s="72">
-        <f t="shared" si="3"/>
-        <v>271</v>
-      </c>
-      <c r="F23" s="71">
-        <f t="shared" si="0"/>
-        <v>-179</v>
-      </c>
-      <c r="H23" s="54"/>
-      <c r="I23" s="45"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="51">
-        <v>17</v>
-      </c>
-      <c r="B24" s="59">
-        <f t="shared" si="2"/>
-        <v>285</v>
-      </c>
-      <c r="C24" s="42">
-        <f t="shared" si="1"/>
-        <v>-191</v>
-      </c>
-      <c r="D24" s="51">
-        <v>17</v>
-      </c>
-      <c r="E24" s="72">
-        <f t="shared" si="3"/>
-        <v>285</v>
-      </c>
-      <c r="F24" s="71">
-        <f t="shared" si="0"/>
-        <v>-193</v>
-      </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="45"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="51">
-        <v>18</v>
-      </c>
-      <c r="B25" s="59">
-        <f t="shared" si="2"/>
-        <v>299</v>
-      </c>
-      <c r="C25" s="42">
-        <f t="shared" si="1"/>
-        <v>-205</v>
-      </c>
-      <c r="D25" s="51">
-        <v>18</v>
-      </c>
-      <c r="E25" s="72">
-        <f t="shared" si="3"/>
-        <v>299</v>
-      </c>
-      <c r="F25" s="71">
-        <f t="shared" si="0"/>
-        <v>-207</v>
-      </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="45"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="51">
-        <v>19</v>
-      </c>
-      <c r="B26" s="59">
-        <f t="shared" si="2"/>
-        <v>313</v>
-      </c>
-      <c r="C26" s="42">
-        <f t="shared" si="1"/>
-        <v>-219</v>
-      </c>
-      <c r="D26" s="51">
-        <v>19</v>
-      </c>
-      <c r="E26" s="72">
-        <f t="shared" si="3"/>
-        <v>313</v>
-      </c>
-      <c r="F26" s="71">
-        <f t="shared" si="0"/>
-        <v>-221</v>
-      </c>
-      <c r="H26" s="54"/>
-      <c r="I26" s="45"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
-        <v>20</v>
-      </c>
-      <c r="B27" s="59">
-        <f t="shared" si="2"/>
-        <v>327</v>
-      </c>
-      <c r="C27" s="42">
-        <f t="shared" si="1"/>
-        <v>-233</v>
-      </c>
-      <c r="D27" s="51">
-        <v>20</v>
-      </c>
-      <c r="E27" s="72">
-        <f t="shared" si="3"/>
-        <v>327</v>
-      </c>
-      <c r="F27" s="71">
-        <f t="shared" si="0"/>
-        <v>-235</v>
-      </c>
-      <c r="H27" s="54"/>
-      <c r="I27" s="45"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="51">
-        <v>21</v>
-      </c>
-      <c r="B28" s="59">
-        <f t="shared" si="2"/>
-        <v>341</v>
-      </c>
-      <c r="C28" s="42">
-        <f t="shared" si="1"/>
-        <v>-247</v>
-      </c>
-      <c r="D28" s="51">
-        <v>21</v>
-      </c>
-      <c r="E28" s="72">
-        <f t="shared" si="3"/>
-        <v>341</v>
-      </c>
-      <c r="F28" s="71">
-        <f t="shared" si="0"/>
-        <v>-249</v>
-      </c>
-      <c r="H28" s="54"/>
-      <c r="I28" s="45"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="51">
-        <v>22</v>
-      </c>
-      <c r="B29" s="59">
-        <f t="shared" si="2"/>
-        <v>355</v>
-      </c>
-      <c r="C29" s="42">
-        <f t="shared" si="1"/>
-        <v>-261</v>
-      </c>
-      <c r="D29" s="51">
-        <v>22</v>
-      </c>
-      <c r="E29" s="72">
-        <f t="shared" si="3"/>
-        <v>355</v>
-      </c>
-      <c r="F29" s="71">
-        <f t="shared" si="0"/>
-        <v>-263</v>
-      </c>
-      <c r="H29" s="54"/>
-      <c r="I29" s="45"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="51">
-        <v>23</v>
-      </c>
-      <c r="B30" s="59">
-        <f t="shared" si="2"/>
-        <v>369</v>
-      </c>
-      <c r="C30" s="42">
-        <f t="shared" si="1"/>
-        <v>-275</v>
-      </c>
-      <c r="D30" s="51">
-        <v>23</v>
-      </c>
-      <c r="E30" s="72">
-        <f t="shared" si="3"/>
-        <v>369</v>
-      </c>
-      <c r="F30" s="71">
-        <f t="shared" si="0"/>
-        <v>-277</v>
-      </c>
-      <c r="H30" s="54"/>
-      <c r="I30" s="45"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="51">
-        <v>24</v>
-      </c>
-      <c r="B31" s="59">
-        <f t="shared" si="2"/>
-        <v>383</v>
-      </c>
-      <c r="C31" s="42">
-        <f t="shared" si="1"/>
-        <v>-289</v>
-      </c>
-      <c r="D31" s="51">
-        <v>24</v>
-      </c>
-      <c r="E31" s="72">
-        <f t="shared" si="3"/>
-        <v>383</v>
-      </c>
-      <c r="F31" s="71">
-        <f t="shared" si="0"/>
-        <v>-291</v>
-      </c>
-      <c r="H31" s="54"/>
-      <c r="I31" s="45"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="51">
-        <v>25</v>
-      </c>
-      <c r="B32" s="59">
-        <f t="shared" si="2"/>
-        <v>397</v>
-      </c>
-      <c r="C32" s="42">
-        <f t="shared" si="1"/>
-        <v>-303</v>
-      </c>
-      <c r="D32" s="51">
-        <v>25</v>
-      </c>
-      <c r="E32" s="72">
-        <f t="shared" si="3"/>
-        <v>397</v>
-      </c>
-      <c r="F32" s="71">
-        <f t="shared" si="0"/>
-        <v>-305</v>
-      </c>
-      <c r="H32" s="54"/>
-      <c r="I32" s="45"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="51">
-        <v>26</v>
-      </c>
-      <c r="B33" s="59">
-        <f t="shared" si="2"/>
-        <v>411</v>
-      </c>
-      <c r="C33" s="42">
-        <f t="shared" si="1"/>
-        <v>-317</v>
-      </c>
-      <c r="D33" s="51">
-        <v>26</v>
-      </c>
-      <c r="E33" s="72">
-        <f t="shared" si="3"/>
-        <v>411</v>
-      </c>
-      <c r="F33" s="71">
-        <f t="shared" si="0"/>
-        <v>-319</v>
-      </c>
-      <c r="H33" s="54"/>
-      <c r="I33" s="45"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="51">
-        <v>27</v>
-      </c>
-      <c r="B34" s="59">
-        <f t="shared" si="2"/>
-        <v>425</v>
-      </c>
-      <c r="C34" s="42">
-        <f t="shared" si="1"/>
-        <v>-331</v>
-      </c>
-      <c r="D34" s="51">
-        <v>27</v>
-      </c>
-      <c r="E34" s="72">
-        <f t="shared" si="3"/>
-        <v>425</v>
-      </c>
-      <c r="F34" s="71">
-        <f t="shared" si="0"/>
-        <v>-333</v>
-      </c>
-      <c r="H34" s="54"/>
-      <c r="I34" s="45"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="51">
-        <v>28</v>
-      </c>
-      <c r="B35" s="59">
-        <f t="shared" si="2"/>
-        <v>439</v>
-      </c>
-      <c r="C35" s="42">
-        <f t="shared" si="1"/>
-        <v>-345</v>
-      </c>
-      <c r="D35" s="51">
-        <v>28</v>
-      </c>
-      <c r="E35" s="72">
-        <f t="shared" si="3"/>
-        <v>439</v>
-      </c>
-      <c r="F35" s="71">
-        <f t="shared" si="0"/>
-        <v>-347</v>
-      </c>
-      <c r="H35" s="54"/>
-      <c r="I35" s="45"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="51">
-        <v>29</v>
-      </c>
-      <c r="B36" s="59">
-        <f t="shared" si="2"/>
-        <v>453</v>
-      </c>
-      <c r="C36" s="42">
-        <f t="shared" si="1"/>
-        <v>-359</v>
-      </c>
-      <c r="D36" s="51">
-        <v>29</v>
-      </c>
-      <c r="E36" s="72">
-        <f t="shared" si="3"/>
-        <v>453</v>
-      </c>
-      <c r="F36" s="71">
-        <f t="shared" si="0"/>
-        <v>-361</v>
-      </c>
-      <c r="H36" s="54"/>
-      <c r="I36" s="45"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="51">
-        <v>30</v>
-      </c>
-      <c r="B37" s="59">
-        <f t="shared" si="2"/>
-        <v>467</v>
-      </c>
-      <c r="C37" s="42">
-        <f t="shared" si="1"/>
-        <v>-373</v>
-      </c>
-      <c r="D37" s="51">
-        <v>30</v>
-      </c>
-      <c r="E37" s="72">
-        <f t="shared" si="3"/>
-        <v>467</v>
-      </c>
-      <c r="F37" s="71">
-        <f t="shared" si="0"/>
-        <v>-375</v>
-      </c>
-      <c r="H37" s="54"/>
-      <c r="I37" s="45"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="51">
-        <v>31</v>
-      </c>
-      <c r="B38" s="59">
-        <f t="shared" si="2"/>
-        <v>481</v>
-      </c>
-      <c r="C38" s="42">
-        <f t="shared" si="1"/>
-        <v>-387</v>
-      </c>
-      <c r="D38" s="51">
-        <v>31</v>
-      </c>
-      <c r="E38" s="72">
-        <f t="shared" si="3"/>
-        <v>481</v>
-      </c>
-      <c r="F38" s="71">
-        <f t="shared" si="0"/>
-        <v>-389</v>
-      </c>
-      <c r="H38" s="54"/>
-      <c r="I38" s="45"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="51">
-        <v>32</v>
-      </c>
-      <c r="B39" s="59">
-        <f t="shared" si="2"/>
-        <v>495</v>
-      </c>
-      <c r="C39" s="42">
-        <f t="shared" si="1"/>
-        <v>-401</v>
-      </c>
-      <c r="D39" s="51">
-        <v>32</v>
-      </c>
-      <c r="E39" s="72">
-        <f t="shared" si="3"/>
-        <v>495</v>
-      </c>
-      <c r="F39" s="71">
-        <f t="shared" si="0"/>
-        <v>-403</v>
-      </c>
-      <c r="H39" s="54"/>
-      <c r="I39" s="45"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="51">
-        <v>33</v>
-      </c>
-      <c r="B40" s="59">
-        <f t="shared" si="2"/>
-        <v>509</v>
-      </c>
-      <c r="C40" s="42">
-        <f t="shared" si="1"/>
-        <v>-415</v>
-      </c>
-      <c r="D40" s="51">
-        <v>33</v>
-      </c>
-      <c r="E40" s="72">
-        <f t="shared" si="3"/>
-        <v>509</v>
-      </c>
-      <c r="F40" s="71">
-        <f t="shared" si="0"/>
-        <v>-417</v>
-      </c>
-      <c r="H40" s="54"/>
-      <c r="I40" s="45"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="51">
-        <v>34</v>
-      </c>
-      <c r="B41" s="59">
-        <f t="shared" si="2"/>
-        <v>523</v>
-      </c>
-      <c r="C41" s="42">
-        <f t="shared" si="1"/>
-        <v>-429</v>
-      </c>
-      <c r="D41" s="51">
-        <v>34</v>
-      </c>
-      <c r="E41" s="72">
-        <f t="shared" si="3"/>
-        <v>523</v>
-      </c>
-      <c r="F41" s="71">
-        <f t="shared" si="0"/>
-        <v>-431</v>
-      </c>
-      <c r="H41" s="54"/>
-      <c r="I41" s="45"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="51">
-        <v>35</v>
-      </c>
-      <c r="B42" s="59">
-        <f t="shared" si="2"/>
-        <v>537</v>
-      </c>
-      <c r="C42" s="42">
-        <f t="shared" si="1"/>
-        <v>-443</v>
-      </c>
-      <c r="D42" s="51">
-        <v>35</v>
-      </c>
-      <c r="E42" s="72">
-        <f t="shared" si="3"/>
-        <v>537</v>
-      </c>
-      <c r="F42" s="71">
-        <f t="shared" si="0"/>
-        <v>-445</v>
-      </c>
-      <c r="H42" s="54"/>
-      <c r="I42" s="45"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="51">
-        <v>36</v>
-      </c>
-      <c r="B43" s="59">
-        <f t="shared" si="2"/>
-        <v>551</v>
-      </c>
-      <c r="C43" s="42">
-        <f t="shared" si="1"/>
-        <v>-457</v>
-      </c>
-      <c r="D43" s="51">
-        <v>36</v>
-      </c>
-      <c r="E43" s="72">
-        <f t="shared" si="3"/>
-        <v>551</v>
-      </c>
-      <c r="F43" s="71">
-        <f t="shared" si="0"/>
-        <v>-459</v>
-      </c>
-      <c r="H43" s="54"/>
-      <c r="I43" s="45"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="51">
-        <v>37</v>
-      </c>
-      <c r="B44" s="59">
-        <f t="shared" si="2"/>
-        <v>565</v>
-      </c>
-      <c r="C44" s="42">
-        <f t="shared" si="1"/>
-        <v>-471</v>
-      </c>
-      <c r="D44" s="51">
-        <v>37</v>
-      </c>
-      <c r="E44" s="72">
-        <f t="shared" si="3"/>
-        <v>565</v>
-      </c>
-      <c r="F44" s="71">
-        <f t="shared" si="0"/>
-        <v>-473</v>
-      </c>
-      <c r="H44" s="54"/>
-      <c r="I44" s="45"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="51">
+        <v>-485</v>
+      </c>
+      <c r="D46" s="50">
         <v>38</v>
       </c>
-      <c r="B45" s="59">
+      <c r="E46" s="67">
         <f t="shared" si="2"/>
         <v>579</v>
       </c>
-      <c r="C45" s="42">
+      <c r="F46" s="66">
+        <f t="shared" si="3"/>
+        <v>-487</v>
+      </c>
+      <c r="G46" s="124">
         <f t="shared" si="1"/>
-        <v>-485</v>
-      </c>
-      <c r="D45" s="51">
-        <v>38</v>
-      </c>
-      <c r="E45" s="72">
-        <f t="shared" si="3"/>
+        <v>-38</v>
+      </c>
+      <c r="H46" s="66">
+        <f>$F$4-E46-94</f>
+        <v>-487</v>
+      </c>
+      <c r="I46" s="57">
+        <f>I$9+(14*D45)</f>
         <v>579</v>
       </c>
-      <c r="F45" s="71">
+      <c r="J46" s="53"/>
+      <c r="K46" s="44"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="50">
+        <v>39</v>
+      </c>
+      <c r="B47" s="57">
+        <f>B$9+(14*A46)</f>
+        <v>593</v>
+      </c>
+      <c r="C47" s="41">
         <f t="shared" si="0"/>
-        <v>-487</v>
-      </c>
-      <c r="H45" s="54"/>
-      <c r="I45" s="45"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="51">
+        <v>-499</v>
+      </c>
+      <c r="D47" s="50">
         <v>39</v>
       </c>
-      <c r="B46" s="59">
+      <c r="E47" s="67">
         <f t="shared" si="2"/>
         <v>593</v>
       </c>
-      <c r="C46" s="42">
+      <c r="F47" s="66">
+        <f t="shared" si="3"/>
+        <v>-501</v>
+      </c>
+      <c r="G47" s="124">
         <f t="shared" si="1"/>
-        <v>-499</v>
-      </c>
-      <c r="D46" s="51">
-        <v>39</v>
-      </c>
-      <c r="E46" s="72">
-        <f t="shared" si="3"/>
+        <v>-39</v>
+      </c>
+      <c r="H47" s="66">
+        <f>$F$4-E47-94</f>
+        <v>-501</v>
+      </c>
+      <c r="I47" s="57">
+        <f>I$9+(14*D46)</f>
         <v>593</v>
       </c>
-      <c r="F46" s="71">
+      <c r="J47" s="53"/>
+      <c r="K47" s="44"/>
+    </row>
+    <row r="48" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="51">
+        <v>40</v>
+      </c>
+      <c r="B48" s="58">
+        <f>B$9+(14*A47)</f>
+        <v>607</v>
+      </c>
+      <c r="C48" s="41">
         <f t="shared" si="0"/>
-        <v>-501</v>
-      </c>
-      <c r="H46" s="54"/>
-      <c r="I46" s="45"/>
-    </row>
-    <row r="47" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="52">
+        <v>-513</v>
+      </c>
+      <c r="D48" s="51">
         <v>40</v>
       </c>
-      <c r="B47" s="60">
+      <c r="E48" s="68">
         <f t="shared" si="2"/>
         <v>607</v>
       </c>
-      <c r="C47" s="42">
+      <c r="F48" s="69">
+        <f t="shared" si="3"/>
+        <v>-515</v>
+      </c>
+      <c r="G48" s="124">
         <f t="shared" si="1"/>
-        <v>-513</v>
-      </c>
-      <c r="D47" s="52">
-        <v>40</v>
-      </c>
-      <c r="E47" s="73">
-        <f t="shared" si="3"/>
+        <v>-40</v>
+      </c>
+      <c r="H48" s="69">
+        <f>$F$4-E48-94</f>
+        <v>-515</v>
+      </c>
+      <c r="I48" s="57">
+        <f>I$9+(14*D47)</f>
         <v>607</v>
       </c>
-      <c r="F47" s="74">
-        <f t="shared" si="0"/>
-        <v>-515</v>
-      </c>
-      <c r="H47" s="55"/>
-      <c r="I47" s="46"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="N1:O1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G9:G48">
+    <sortCondition descending="1" ref="G8:G48"/>
+  </sortState>
+  <mergeCells count="15">
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8:B47">
-    <cfRule type="expression" dxfId="11" priority="4">
-      <formula>(1+ ((B8-61)/14)) &gt; $B$2</formula>
+  <conditionalFormatting sqref="B9:B48">
+    <cfRule type="expression" dxfId="15" priority="12">
+      <formula>(1+ ((B9-61)/14)) &gt; $B$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C47">
-    <cfRule type="expression" dxfId="10" priority="5">
-      <formula>B8&gt;C8</formula>
+  <conditionalFormatting sqref="C9:C48">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>B9&gt;C9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E47">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>(1+ ((E8-61)/14)) &gt; $B$2</formula>
+  <conditionalFormatting sqref="E9:E48">
+    <cfRule type="expression" dxfId="13" priority="10">
+      <formula>(1+ ((E9-61)/14)) &gt; $B$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F5">
-    <cfRule type="expression" dxfId="8" priority="16">
+  <conditionalFormatting sqref="F3:I5">
+    <cfRule type="expression" dxfId="12" priority="24">
       <formula>COUNTIF($B$2,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:F47">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>(1+ ((ABS(F8-$F$4)-61)/14)) &gt; $B$2</formula>
+  <conditionalFormatting sqref="F9:F48">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>(1+ ((ABS(F9-$F$4)-61)/14)) &gt; $B$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10 G12">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>COUNTIF($G$8,"")</formula>
+  <conditionalFormatting sqref="I9:I48">
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>(1+ ((I9-61)/14)) &gt; $B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9:G48">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:H48">
+    <cfRule type="expression" dxfId="9" priority="2">
+      <formula>(1+ ((ABS(H9-$F$4)-61)/14)) &gt; $B$2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydrocarbon chain length" prompt="Enter a whole number (greater than 1) indicating the number of carbons in the hydrocarbon chain of your target compound." sqref="B2" xr:uid="{F7014332-3719-4885-95BF-44AFD9FD41C8}">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Information display cell" prompt="Do not modify the content of this cell!_x000a_" sqref="F3:F5" xr:uid="{21ECB7F2-771B-4437-8B65-3F0ADFF96332}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Information display cell" prompt="Do not modify the content of this cell!_x000a_" sqref="F3:I5" xr:uid="{21ECB7F2-771B-4437-8B65-3F0ADFF96332}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>